<commit_message>
Indexant llibre Blancafort anys 1919 - 1952
</commit_message>
<xml_diff>
--- a/Bisbats/Catalunya/Lleida/Blancafort/Sacraments/Baptismes/Excel/Baptismes_Parroquia_Blancafort.xlsx
+++ b/Bisbats/Catalunya/Lleida/Blancafort/Sacraments/Baptismes/Excel/Baptismes_Parroquia_Blancafort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vstudio-code\repositorisArbre\DadesGenerals\Bisbats\Catalunya\Lleida\Blancafort\Sacraments\Baptismes\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC71DD6-F407-453A-B63A-4515E21231E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859C1A04-8637-4F28-9B9B-CCC25462FEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
   <si>
     <t>Cognoms</t>
   </si>
@@ -100,6 +100,51 @@
   </si>
   <si>
     <t>Farré Ludriga</t>
+  </si>
+  <si>
+    <t>Gracia Jubillà</t>
+  </si>
+  <si>
+    <t>Bendicho Jubilla</t>
+  </si>
+  <si>
+    <t>Gessé Eguanito</t>
+  </si>
+  <si>
+    <t>Benavarre Gessé</t>
+  </si>
+  <si>
+    <t>Gessé Álvarez</t>
+  </si>
+  <si>
+    <t>Bendicho Jubillá</t>
+  </si>
+  <si>
+    <t>Gessé Ros</t>
+  </si>
+  <si>
+    <t>Cunyat Vigo</t>
+  </si>
+  <si>
+    <t>Gessé Àlbarez</t>
+  </si>
+  <si>
+    <t>Benabarre Gessé</t>
+  </si>
+  <si>
+    <t>Fontelles Gessé</t>
+  </si>
+  <si>
+    <t>FALTA</t>
+  </si>
+  <si>
+    <t>Puig Montanuy</t>
+  </si>
+  <si>
+    <t>Farré Tolsà</t>
+  </si>
+  <si>
+    <t>Gessé Jubillà</t>
   </si>
 </sst>
 </file>
@@ -430,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,6 +691,368 @@
         <v>1924</v>
       </c>
     </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>11</v>
+      </c>
+      <c r="C20">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <v>1927</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>14</v>
+      </c>
+      <c r="C24">
+        <v>1927</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>14</v>
+      </c>
+      <c r="C25">
+        <v>1928</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <v>15</v>
+      </c>
+      <c r="C26">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27">
+        <v>15</v>
+      </c>
+      <c r="C27">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28">
+        <v>16</v>
+      </c>
+      <c r="C28">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>17</v>
+      </c>
+      <c r="C29">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>17</v>
+      </c>
+      <c r="C30">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31">
+        <v>18</v>
+      </c>
+      <c r="C31">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>19</v>
+      </c>
+      <c r="C32">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33">
+        <v>20</v>
+      </c>
+      <c r="C33">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>20</v>
+      </c>
+      <c r="C34">
+        <v>1933</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>21</v>
+      </c>
+      <c r="C35">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>23</v>
+      </c>
+      <c r="C37">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>25</v>
+      </c>
+      <c r="C39">
+        <v>1938</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40">
+        <v>25</v>
+      </c>
+      <c r="C40">
+        <v>1939</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41">
+        <v>26</v>
+      </c>
+      <c r="C41">
+        <v>1942</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42">
+        <v>27</v>
+      </c>
+      <c r="C42">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45">
+        <v>30</v>
+      </c>
+      <c r="C45">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46">
+        <v>31</v>
+      </c>
+      <c r="C46">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47">
+        <v>32</v>
+      </c>
+      <c r="C47">
+        <v>1952</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
afegint dades Llibres Baptisme Blancafort
</commit_message>
<xml_diff>
--- a/Bisbats/Catalunya/Lleida/Blancafort/Sacraments/Baptismes/Excel/Baptismes_Parroquia_Blancafort.xlsx
+++ b/Bisbats/Catalunya/Lleida/Blancafort/Sacraments/Baptismes/Excel/Baptismes_Parroquia_Blancafort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vstudio-code\repositorisArbre\DadesGenerals\Bisbats\Catalunya\Lleida\Blancafort\Sacraments\Baptismes\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC60CF3B-2615-46E6-B70B-2C9493E4B601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BA46EF-6438-41C0-90DA-E5A3B24880D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="214">
   <si>
     <t>Cognoms</t>
   </si>
@@ -93,6 +93,9 @@
     <t>Millorable</t>
   </si>
   <si>
+    <t>Ensenyat Gessé</t>
+  </si>
+  <si>
     <t>Ensenyat Vigo</t>
   </si>
   <si>
@@ -619,6 +622,54 @@
   </si>
   <si>
     <t>Gessé Saurí</t>
+  </si>
+  <si>
+    <t>Gessé Gessé Jaume Francisco</t>
+  </si>
+  <si>
+    <t>Nadal Pociello Pau Salbador Josep</t>
+  </si>
+  <si>
+    <t>Jubilla Gras</t>
+  </si>
+  <si>
+    <t>Borrosa</t>
+  </si>
+  <si>
+    <t>Gessé Cires</t>
+  </si>
+  <si>
+    <t>Gessé Masana</t>
+  </si>
+  <si>
+    <t>Gessé Gessé Antoni Agusti</t>
+  </si>
+  <si>
+    <t>12/04/1878</t>
+  </si>
+  <si>
+    <t>10/04/1878</t>
+  </si>
+  <si>
+    <t>Andreu Tagries?</t>
+  </si>
+  <si>
+    <t>Gessé Pijuan</t>
+  </si>
+  <si>
+    <t>Mateu Badia</t>
+  </si>
+  <si>
+    <t>Gessé Massana</t>
+  </si>
+  <si>
+    <t>Bendicho Salse</t>
+  </si>
+  <si>
+    <t>Gessé Gessé Dolors Rosa</t>
+  </si>
+  <si>
+    <t>15/12/1880</t>
   </si>
 </sst>
 </file>
@@ -953,11 +1004,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q254"/>
+  <dimension ref="A1:Q289"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A225" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C252" sqref="C252:C254"/>
+      <pane ySplit="1" topLeftCell="A259" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A290" sqref="A290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,7 +1094,7 @@
         <v>1919</v>
       </c>
       <c r="P2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Q2" t="s">
         <v>19</v>
@@ -1060,7 +1111,7 @@
         <v>1920</v>
       </c>
       <c r="P3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Q3" t="s">
         <v>19</v>
@@ -1077,7 +1128,7 @@
         <v>1921</v>
       </c>
       <c r="P4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Q4" t="s">
         <v>20</v>
@@ -1094,7 +1145,7 @@
         <v>1922</v>
       </c>
       <c r="P5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Q5" t="s">
         <v>20</v>
@@ -1102,7 +1153,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -1111,12 +1162,12 @@
         <v>1922</v>
       </c>
       <c r="P6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -1125,12 +1176,12 @@
         <v>1922</v>
       </c>
       <c r="P7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -1139,12 +1190,12 @@
         <v>1922</v>
       </c>
       <c r="P8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -1153,7 +1204,7 @@
         <v>1922</v>
       </c>
       <c r="P9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -1167,12 +1218,12 @@
         <v>1923</v>
       </c>
       <c r="P10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -1181,12 +1232,12 @@
         <v>1923</v>
       </c>
       <c r="P11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12">
         <v>7</v>
@@ -1195,12 +1246,12 @@
         <v>1923</v>
       </c>
       <c r="P12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>7</v>
@@ -1209,12 +1260,12 @@
         <v>1924</v>
       </c>
       <c r="P13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -1223,7 +1274,7 @@
         <v>1924</v>
       </c>
       <c r="P14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1237,12 +1288,12 @@
         <v>1924</v>
       </c>
       <c r="P15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16">
         <v>9</v>
@@ -1251,12 +1302,12 @@
         <v>1925</v>
       </c>
       <c r="P16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17">
         <v>10</v>
@@ -1265,12 +1316,12 @@
         <v>1925</v>
       </c>
       <c r="P17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18">
         <v>10</v>
@@ -1279,12 +1330,12 @@
         <v>1925</v>
       </c>
       <c r="P18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>11</v>
@@ -1293,12 +1344,12 @@
         <v>1925</v>
       </c>
       <c r="P19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20">
         <v>11</v>
@@ -1307,12 +1358,12 @@
         <v>1925</v>
       </c>
       <c r="P20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>12</v>
@@ -1321,12 +1372,12 @@
         <v>1926</v>
       </c>
       <c r="P21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B22">
         <v>12</v>
@@ -1335,12 +1386,12 @@
         <v>1926</v>
       </c>
       <c r="P22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23">
         <v>13</v>
@@ -1349,12 +1400,12 @@
         <v>1927</v>
       </c>
       <c r="P23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>14</v>
@@ -1363,12 +1414,12 @@
         <v>1927</v>
       </c>
       <c r="P24" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>14</v>
@@ -1377,12 +1428,12 @@
         <v>1928</v>
       </c>
       <c r="P25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B26">
         <v>15</v>
@@ -1391,12 +1442,12 @@
         <v>1929</v>
       </c>
       <c r="P26" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B27">
         <v>15</v>
@@ -1405,12 +1456,12 @@
         <v>1929</v>
       </c>
       <c r="P27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B28">
         <v>16</v>
@@ -1419,12 +1470,12 @@
         <v>1929</v>
       </c>
       <c r="P28" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B29">
         <v>17</v>
@@ -1433,12 +1484,12 @@
         <v>1929</v>
       </c>
       <c r="P29" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B30">
         <v>17</v>
@@ -1447,12 +1498,12 @@
         <v>1929</v>
       </c>
       <c r="P30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B31">
         <v>18</v>
@@ -1461,12 +1512,12 @@
         <v>1930</v>
       </c>
       <c r="P31" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B32">
         <v>19</v>
@@ -1475,12 +1526,12 @@
         <v>1930</v>
       </c>
       <c r="P32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B33">
         <v>20</v>
@@ -1489,12 +1540,12 @@
         <v>1932</v>
       </c>
       <c r="P33" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34">
         <v>20</v>
@@ -1503,12 +1554,12 @@
         <v>1933</v>
       </c>
       <c r="P34" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35">
         <v>21</v>
@@ -1517,23 +1568,23 @@
         <v>1934</v>
       </c>
       <c r="P35" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B36">
         <v>22</v>
       </c>
       <c r="P36" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37">
         <v>23</v>
@@ -1542,23 +1593,23 @@
         <v>1936</v>
       </c>
       <c r="P37" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38">
         <v>24</v>
       </c>
       <c r="P38" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39">
         <v>25</v>
@@ -1567,12 +1618,12 @@
         <v>1938</v>
       </c>
       <c r="P39" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B40">
         <v>25</v>
@@ -1581,12 +1632,12 @@
         <v>1939</v>
       </c>
       <c r="P40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41">
         <v>26</v>
@@ -1595,12 +1646,12 @@
         <v>1942</v>
       </c>
       <c r="P41" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B42">
         <v>27</v>
@@ -1609,34 +1660,34 @@
         <v>1944</v>
       </c>
       <c r="P42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B43">
         <v>28</v>
       </c>
       <c r="P43" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B44">
         <v>29</v>
       </c>
       <c r="P44" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B45">
         <v>30</v>
@@ -1645,12 +1696,12 @@
         <v>1947</v>
       </c>
       <c r="P45" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B46">
         <v>31</v>
@@ -1659,12 +1710,12 @@
         <v>1950</v>
       </c>
       <c r="P46" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B47">
         <v>32</v>
@@ -1673,12 +1724,12 @@
         <v>1952</v>
       </c>
       <c r="P47" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -1687,12 +1738,12 @@
         <v>1896</v>
       </c>
       <c r="P48" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -1701,12 +1752,12 @@
         <v>1896</v>
       </c>
       <c r="P49" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -1715,36 +1766,36 @@
         <v>1897</v>
       </c>
       <c r="D50" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" t="s">
+        <v>74</v>
+      </c>
+      <c r="F50" t="s">
         <v>48</v>
       </c>
-      <c r="E50" t="s">
-        <v>73</v>
-      </c>
-      <c r="F50" t="s">
-        <v>47</v>
-      </c>
       <c r="G50" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I50" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J50" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K50" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P50" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -1753,12 +1804,12 @@
         <v>1897</v>
       </c>
       <c r="P51" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B52">
         <v>3</v>
@@ -1767,12 +1818,12 @@
         <v>1897</v>
       </c>
       <c r="P52" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B53">
         <v>3</v>
@@ -1781,12 +1832,12 @@
         <v>1897</v>
       </c>
       <c r="P53" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -1795,12 +1846,12 @@
         <v>1897</v>
       </c>
       <c r="P54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -1809,12 +1860,12 @@
         <v>1897</v>
       </c>
       <c r="P55" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B56">
         <v>5</v>
@@ -1823,12 +1874,12 @@
         <v>1897</v>
       </c>
       <c r="P56" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B57">
         <v>5</v>
@@ -1837,12 +1888,12 @@
         <v>1898</v>
       </c>
       <c r="P57" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B58">
         <v>6</v>
@@ -1851,36 +1902,36 @@
         <v>1898</v>
       </c>
       <c r="D58" t="s">
+        <v>49</v>
+      </c>
+      <c r="E58" t="s">
+        <v>74</v>
+      </c>
+      <c r="F58" t="s">
         <v>48</v>
       </c>
-      <c r="E58" t="s">
-        <v>73</v>
-      </c>
-      <c r="F58" t="s">
-        <v>47</v>
-      </c>
       <c r="G58" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I58" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J58" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K58" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P58" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B59">
         <v>6</v>
@@ -1889,12 +1940,12 @@
         <v>1898</v>
       </c>
       <c r="P59" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B60">
         <v>7</v>
@@ -1903,12 +1954,12 @@
         <v>1899</v>
       </c>
       <c r="P60" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B61">
         <v>7</v>
@@ -1917,12 +1968,12 @@
         <v>1899</v>
       </c>
       <c r="P61" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -1931,12 +1982,12 @@
         <v>1899</v>
       </c>
       <c r="P62" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -1945,12 +1996,12 @@
         <v>1899</v>
       </c>
       <c r="P63" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B64">
         <v>9</v>
@@ -1959,12 +2010,12 @@
         <v>1900</v>
       </c>
       <c r="P64" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B65">
         <v>10</v>
@@ -1973,39 +2024,39 @@
         <v>1900</v>
       </c>
       <c r="D65" t="s">
+        <v>49</v>
+      </c>
+      <c r="E65" t="s">
+        <v>74</v>
+      </c>
+      <c r="F65" t="s">
         <v>48</v>
       </c>
-      <c r="E65" t="s">
-        <v>73</v>
-      </c>
-      <c r="F65" t="s">
-        <v>47</v>
-      </c>
       <c r="G65" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H65" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I65" s="3">
         <v>109</v>
       </c>
       <c r="J65" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K65" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L65" s="3">
         <v>110</v>
       </c>
       <c r="P65" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B66">
         <v>11</v>
@@ -2014,12 +2065,12 @@
         <v>1900</v>
       </c>
       <c r="P66" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B67">
         <v>12</v>
@@ -2028,12 +2079,12 @@
         <v>1900</v>
       </c>
       <c r="P67" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B68">
         <v>12</v>
@@ -2042,12 +2093,12 @@
         <v>1900</v>
       </c>
       <c r="P68" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B69">
         <v>13</v>
@@ -2056,12 +2107,12 @@
         <v>1901</v>
       </c>
       <c r="P69" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B70">
         <v>14</v>
@@ -2070,12 +2121,12 @@
         <v>1901</v>
       </c>
       <c r="P70" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B71">
         <v>14</v>
@@ -2084,12 +2135,12 @@
         <v>1901</v>
       </c>
       <c r="P71" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B72">
         <v>15</v>
@@ -2098,12 +2149,12 @@
         <v>1901</v>
       </c>
       <c r="P72" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B73">
         <v>15</v>
@@ -2112,12 +2163,12 @@
         <v>1901</v>
       </c>
       <c r="P73" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B74">
         <v>16</v>
@@ -2126,12 +2177,12 @@
         <v>1901</v>
       </c>
       <c r="P74" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B75">
         <v>17</v>
@@ -2140,12 +2191,12 @@
         <v>1901</v>
       </c>
       <c r="P75" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B76">
         <v>17</v>
@@ -2154,36 +2205,36 @@
         <v>1902</v>
       </c>
       <c r="D76" t="s">
+        <v>49</v>
+      </c>
+      <c r="E76" t="s">
+        <v>74</v>
+      </c>
+      <c r="F76" t="s">
         <v>48</v>
       </c>
-      <c r="E76" t="s">
-        <v>73</v>
-      </c>
-      <c r="F76" t="s">
-        <v>47</v>
-      </c>
       <c r="G76" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I76" s="3">
         <v>747</v>
       </c>
       <c r="J76" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K76" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L76" s="3">
         <v>750</v>
       </c>
       <c r="P76" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B77">
         <v>18</v>
@@ -2192,12 +2243,12 @@
         <v>1902</v>
       </c>
       <c r="P77" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B78">
         <v>19</v>
@@ -2206,12 +2257,12 @@
         <v>1902</v>
       </c>
       <c r="P78" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B79">
         <v>19</v>
@@ -2220,12 +2271,12 @@
         <v>1902</v>
       </c>
       <c r="P79" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B80">
         <v>20</v>
@@ -2234,39 +2285,39 @@
         <v>1902</v>
       </c>
       <c r="D80" t="s">
+        <v>49</v>
+      </c>
+      <c r="E80" t="s">
+        <v>74</v>
+      </c>
+      <c r="F80" t="s">
         <v>48</v>
       </c>
-      <c r="E80" t="s">
-        <v>73</v>
-      </c>
-      <c r="F80" t="s">
-        <v>47</v>
-      </c>
       <c r="G80" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H80" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I80" s="3">
         <v>1093</v>
       </c>
       <c r="J80" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K80" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L80" s="3">
         <v>1096</v>
       </c>
       <c r="P80" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B81">
         <v>20</v>
@@ -2275,12 +2326,12 @@
         <v>1903</v>
       </c>
       <c r="P81" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B82">
         <v>21</v>
@@ -2289,12 +2340,12 @@
         <v>1903</v>
       </c>
       <c r="P82" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B83">
         <v>22</v>
@@ -2303,12 +2354,12 @@
         <v>1903</v>
       </c>
       <c r="P83" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B84">
         <v>22</v>
@@ -2317,12 +2368,12 @@
         <v>1903</v>
       </c>
       <c r="P84" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B85">
         <v>23</v>
@@ -2331,12 +2382,12 @@
         <v>1903</v>
       </c>
       <c r="P85" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B86">
         <v>24</v>
@@ -2345,12 +2396,12 @@
         <v>1904</v>
       </c>
       <c r="P86" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B87">
         <v>24</v>
@@ -2359,12 +2410,12 @@
         <v>1904</v>
       </c>
       <c r="P87" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B88">
         <v>25</v>
@@ -2373,12 +2424,12 @@
         <v>1904</v>
       </c>
       <c r="P88" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B89">
         <v>26</v>
@@ -2387,12 +2438,12 @@
         <v>1904</v>
       </c>
       <c r="P89" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B90">
         <v>26</v>
@@ -2401,12 +2452,12 @@
         <v>1904</v>
       </c>
       <c r="P90" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B91">
         <v>27</v>
@@ -2415,12 +2466,12 @@
         <v>1904</v>
       </c>
       <c r="P91" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B92">
         <v>27</v>
@@ -2429,12 +2480,12 @@
         <v>1905</v>
       </c>
       <c r="P92" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B93">
         <v>28</v>
@@ -2443,33 +2494,33 @@
         <v>1905</v>
       </c>
       <c r="D93" t="s">
+        <v>49</v>
+      </c>
+      <c r="E93" t="s">
+        <v>74</v>
+      </c>
+      <c r="F93" t="s">
         <v>48</v>
       </c>
-      <c r="E93" t="s">
-        <v>73</v>
-      </c>
-      <c r="F93" t="s">
-        <v>47</v>
-      </c>
       <c r="G93" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I93" s="3">
         <v>1917</v>
       </c>
       <c r="J93" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L93" s="3">
         <v>1919</v>
       </c>
       <c r="P93" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B94">
         <v>28</v>
@@ -2478,33 +2529,33 @@
         <v>1905</v>
       </c>
       <c r="D94" t="s">
+        <v>49</v>
+      </c>
+      <c r="E94" t="s">
+        <v>74</v>
+      </c>
+      <c r="F94" t="s">
         <v>48</v>
       </c>
-      <c r="E94" t="s">
-        <v>73</v>
-      </c>
-      <c r="F94" t="s">
-        <v>47</v>
-      </c>
       <c r="G94" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I94" s="3">
         <v>1917</v>
       </c>
       <c r="K94" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L94" s="3">
         <v>1919</v>
       </c>
       <c r="P94" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B95">
         <v>29</v>
@@ -2513,12 +2564,12 @@
         <v>1905</v>
       </c>
       <c r="P95" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B96">
         <v>29</v>
@@ -2527,12 +2578,12 @@
         <v>1905</v>
       </c>
       <c r="P96" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B97">
         <v>30</v>
@@ -2541,12 +2592,12 @@
         <v>1906</v>
       </c>
       <c r="P97" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B98">
         <v>31</v>
@@ -2555,12 +2606,12 @@
         <v>1906</v>
       </c>
       <c r="P98" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B99">
         <v>31</v>
@@ -2569,12 +2620,12 @@
         <v>1906</v>
       </c>
       <c r="P99" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B100">
         <v>32</v>
@@ -2583,15 +2634,15 @@
         <v>1906</v>
       </c>
       <c r="P100" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="Q100" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B101">
         <v>33</v>
@@ -2600,12 +2651,12 @@
         <v>1905</v>
       </c>
       <c r="P101" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B102">
         <v>33</v>
@@ -2614,36 +2665,36 @@
         <v>1907</v>
       </c>
       <c r="D102" t="s">
+        <v>49</v>
+      </c>
+      <c r="E102" t="s">
+        <v>74</v>
+      </c>
+      <c r="F102" t="s">
         <v>48</v>
       </c>
-      <c r="E102" t="s">
-        <v>73</v>
-      </c>
-      <c r="F102" t="s">
-        <v>47</v>
-      </c>
       <c r="G102" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I102" s="3">
         <v>2685</v>
       </c>
       <c r="J102" t="s">
+        <v>94</v>
+      </c>
+      <c r="K102" t="s">
         <v>93</v>
-      </c>
-      <c r="K102" t="s">
-        <v>92</v>
       </c>
       <c r="L102" s="3">
         <v>2687</v>
       </c>
       <c r="P102" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B103">
         <v>34</v>
@@ -2652,12 +2703,12 @@
         <v>1907</v>
       </c>
       <c r="P103" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B104">
         <v>35</v>
@@ -2666,12 +2717,12 @@
         <v>1907</v>
       </c>
       <c r="P104" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B105">
         <v>36</v>
@@ -2680,26 +2731,26 @@
         <v>1907</v>
       </c>
       <c r="P105" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C106">
         <v>1931</v>
       </c>
       <c r="P106" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B107">
         <v>37</v>
@@ -2708,12 +2759,12 @@
         <v>1907</v>
       </c>
       <c r="P107" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B108">
         <v>37</v>
@@ -2722,12 +2773,12 @@
         <v>1907</v>
       </c>
       <c r="P108" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B109">
         <v>38</v>
@@ -2736,12 +2787,12 @@
         <v>1907</v>
       </c>
       <c r="P109" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B110">
         <v>39</v>
@@ -2750,12 +2801,12 @@
         <v>1908</v>
       </c>
       <c r="P110" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B111">
         <v>40</v>
@@ -2764,12 +2815,12 @@
         <v>1908</v>
       </c>
       <c r="P111" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B112">
         <v>40</v>
@@ -2778,12 +2829,12 @@
         <v>1908</v>
       </c>
       <c r="P112" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B113">
         <v>41</v>
@@ -2792,36 +2843,36 @@
         <v>1909</v>
       </c>
       <c r="D113" t="s">
+        <v>49</v>
+      </c>
+      <c r="E113" t="s">
+        <v>74</v>
+      </c>
+      <c r="F113" t="s">
         <v>48</v>
       </c>
-      <c r="E113" t="s">
-        <v>73</v>
-      </c>
-      <c r="F113" t="s">
-        <v>47</v>
-      </c>
       <c r="G113" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I113" s="3">
         <v>3603</v>
       </c>
       <c r="J113" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K113" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L113" s="3">
         <v>3611</v>
       </c>
       <c r="P113" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B114">
         <v>42</v>
@@ -2830,12 +2881,12 @@
         <v>1909</v>
       </c>
       <c r="P114" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B115">
         <v>42</v>
@@ -2844,12 +2895,12 @@
         <v>1910</v>
       </c>
       <c r="P115" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B116">
         <v>43</v>
@@ -2858,12 +2909,12 @@
         <v>1910</v>
       </c>
       <c r="P116" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B117">
         <v>44</v>
@@ -2872,12 +2923,12 @@
         <v>1910</v>
       </c>
       <c r="P117" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B118">
         <v>45</v>
@@ -2886,12 +2937,12 @@
         <v>1911</v>
       </c>
       <c r="P118" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B119">
         <v>46</v>
@@ -2900,12 +2951,12 @@
         <v>1911</v>
       </c>
       <c r="P119" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B120">
         <v>46</v>
@@ -2914,12 +2965,12 @@
         <v>1911</v>
       </c>
       <c r="P120" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B121">
         <v>47</v>
@@ -2928,12 +2979,12 @@
         <v>1911</v>
       </c>
       <c r="P121" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B122">
         <v>48</v>
@@ -2942,15 +2993,15 @@
         <v>1912</v>
       </c>
       <c r="P122" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="Q122" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B123">
         <v>48</v>
@@ -2959,12 +3010,12 @@
         <v>1912</v>
       </c>
       <c r="P123" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B124">
         <v>49</v>
@@ -2973,39 +3024,39 @@
         <v>1912</v>
       </c>
       <c r="D124" t="s">
+        <v>49</v>
+      </c>
+      <c r="E124" t="s">
+        <v>74</v>
+      </c>
+      <c r="F124" t="s">
         <v>48</v>
       </c>
-      <c r="E124" t="s">
-        <v>73</v>
-      </c>
-      <c r="F124" t="s">
-        <v>47</v>
-      </c>
       <c r="G124" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H124" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I124" s="3">
         <v>4501</v>
       </c>
       <c r="J124" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K124" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L124" s="3">
         <v>4502</v>
       </c>
       <c r="P124" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B125">
         <v>50</v>
@@ -3014,12 +3065,12 @@
         <v>1912</v>
       </c>
       <c r="P125" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B126">
         <v>51</v>
@@ -3028,12 +3079,12 @@
         <v>1914</v>
       </c>
       <c r="P126" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B127">
         <v>52</v>
@@ -3042,12 +3093,12 @@
         <v>1914</v>
       </c>
       <c r="P127" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B128">
         <v>53</v>
@@ -3056,12 +3107,12 @@
         <v>1914</v>
       </c>
       <c r="P128" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B129">
         <v>53</v>
@@ -3070,36 +3121,36 @@
         <v>1915</v>
       </c>
       <c r="D129" t="s">
+        <v>49</v>
+      </c>
+      <c r="E129" t="s">
+        <v>74</v>
+      </c>
+      <c r="F129" t="s">
         <v>48</v>
       </c>
-      <c r="E129" t="s">
-        <v>73</v>
-      </c>
-      <c r="F129" t="s">
-        <v>47</v>
-      </c>
       <c r="G129" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I129" s="3">
         <v>5734</v>
       </c>
       <c r="J129" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K129" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="L129" s="3">
         <v>5735</v>
       </c>
       <c r="P129" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B130">
         <v>54</v>
@@ -3108,12 +3159,12 @@
         <v>1915</v>
       </c>
       <c r="P130" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B131">
         <v>1</v>
@@ -3122,12 +3173,12 @@
         <v>1852</v>
       </c>
       <c r="P131" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -3138,7 +3189,7 @@
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B133">
         <v>1</v>
@@ -3149,7 +3200,7 @@
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B134">
         <v>2</v>
@@ -3160,7 +3211,7 @@
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B135">
         <v>2</v>
@@ -3171,7 +3222,7 @@
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B136">
         <v>3</v>
@@ -3182,7 +3233,7 @@
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B137">
         <v>3</v>
@@ -3193,15 +3244,15 @@
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B139">
         <v>4</v>
@@ -3212,7 +3263,7 @@
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B140">
         <v>4</v>
@@ -3223,7 +3274,7 @@
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B141">
         <v>4</v>
@@ -3234,7 +3285,7 @@
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B142">
         <v>5</v>
@@ -3245,7 +3296,7 @@
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B143">
         <v>5</v>
@@ -3256,7 +3307,7 @@
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B144">
         <v>6</v>
@@ -3267,7 +3318,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B145">
         <v>6</v>
@@ -3278,7 +3329,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B146">
         <v>6</v>
@@ -3289,7 +3340,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B147">
         <v>7</v>
@@ -3300,7 +3351,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B148">
         <v>7</v>
@@ -3311,7 +3362,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B149">
         <v>8</v>
@@ -3322,7 +3373,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B150">
         <v>8</v>
@@ -3333,7 +3384,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B151">
         <v>8</v>
@@ -3344,7 +3395,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B152">
         <v>9</v>
@@ -3355,7 +3406,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B153">
         <v>9</v>
@@ -3366,7 +3417,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B154">
         <v>9</v>
@@ -3377,7 +3428,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B155">
         <v>10</v>
@@ -3388,7 +3439,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B156">
         <v>10</v>
@@ -3399,7 +3450,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B157">
         <v>10</v>
@@ -3410,7 +3461,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B158">
         <v>11</v>
@@ -3421,7 +3472,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B159">
         <v>11</v>
@@ -3432,7 +3483,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B160">
         <v>12</v>
@@ -3443,7 +3494,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B161">
         <v>12</v>
@@ -3454,7 +3505,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B162">
         <v>13</v>
@@ -3465,7 +3516,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B163">
         <v>13</v>
@@ -3476,7 +3527,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B164">
         <v>14</v>
@@ -3487,7 +3538,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B165">
         <v>15</v>
@@ -3498,7 +3549,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B166">
         <v>16</v>
@@ -3509,7 +3560,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B167">
         <v>16</v>
@@ -3520,7 +3571,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B168">
         <v>16</v>
@@ -3531,7 +3582,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B169">
         <v>17</v>
@@ -3542,7 +3593,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B170">
         <v>17</v>
@@ -3553,7 +3604,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B171">
         <v>18</v>
@@ -3564,7 +3615,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B172">
         <v>18</v>
@@ -3575,7 +3626,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B173">
         <v>19</v>
@@ -3586,7 +3637,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B174">
         <v>19</v>
@@ -3597,7 +3648,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B175">
         <v>20</v>
@@ -3608,7 +3659,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B176">
         <v>20</v>
@@ -3619,7 +3670,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B177">
         <v>20</v>
@@ -3630,7 +3681,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B178">
         <v>21</v>
@@ -3641,7 +3692,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B179">
         <v>21</v>
@@ -3652,7 +3703,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B180">
         <v>22</v>
@@ -3663,7 +3714,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B181">
         <v>22</v>
@@ -3674,7 +3725,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B182">
         <v>22</v>
@@ -3685,7 +3736,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B183">
         <v>23</v>
@@ -3696,7 +3747,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B184">
         <v>23</v>
@@ -3707,7 +3758,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B185">
         <v>24</v>
@@ -3718,7 +3769,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B186">
         <v>24</v>
@@ -3729,7 +3780,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B187">
         <v>25</v>
@@ -3740,7 +3791,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B188">
         <v>25</v>
@@ -3751,7 +3802,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B189">
         <v>26</v>
@@ -3762,7 +3813,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B190">
         <v>26</v>
@@ -3773,7 +3824,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B191">
         <v>27</v>
@@ -3784,7 +3835,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B192">
         <v>27</v>
@@ -3795,7 +3846,7 @@
     </row>
     <row r="193" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B193">
         <v>28</v>
@@ -3806,7 +3857,7 @@
     </row>
     <row r="194" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B194">
         <v>28</v>
@@ -3817,7 +3868,7 @@
     </row>
     <row r="195" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B195">
         <v>29</v>
@@ -3828,7 +3879,7 @@
     </row>
     <row r="196" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B196">
         <v>29</v>
@@ -3837,33 +3888,33 @@
         <v>1863</v>
       </c>
       <c r="D196" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E196" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F196" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G196" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I196" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J196" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K196" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L196" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B197">
         <v>30</v>
@@ -3874,7 +3925,7 @@
     </row>
     <row r="198" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B198">
         <v>30</v>
@@ -3885,7 +3936,7 @@
     </row>
     <row r="199" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B199">
         <v>31</v>
@@ -3896,7 +3947,7 @@
     </row>
     <row r="200" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B200">
         <v>31</v>
@@ -3907,7 +3958,7 @@
     </row>
     <row r="201" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B201">
         <v>32</v>
@@ -3918,7 +3969,7 @@
     </row>
     <row r="202" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B202">
         <v>32</v>
@@ -3929,7 +3980,7 @@
     </row>
     <row r="203" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B203">
         <v>32</v>
@@ -3940,7 +3991,7 @@
     </row>
     <row r="204" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B204">
         <v>33</v>
@@ -3951,7 +4002,7 @@
     </row>
     <row r="205" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B205">
         <v>33</v>
@@ -3962,7 +4013,7 @@
     </row>
     <row r="206" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B206">
         <v>33</v>
@@ -3973,7 +4024,7 @@
     </row>
     <row r="207" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B207">
         <v>34</v>
@@ -3984,7 +4035,7 @@
     </row>
     <row r="208" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B208">
         <v>34</v>
@@ -3993,33 +4044,33 @@
         <v>1866</v>
       </c>
       <c r="D208" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E208" t="s">
+        <v>173</v>
+      </c>
+      <c r="F208" t="s">
+        <v>171</v>
+      </c>
+      <c r="G208" t="s">
+        <v>147</v>
+      </c>
+      <c r="I208" t="s">
+        <v>152</v>
+      </c>
+      <c r="J208" t="s">
+        <v>148</v>
+      </c>
+      <c r="K208" t="s">
         <v>172</v>
       </c>
-      <c r="F208" t="s">
-        <v>170</v>
-      </c>
-      <c r="G208" t="s">
-        <v>146</v>
-      </c>
-      <c r="I208" t="s">
-        <v>151</v>
-      </c>
-      <c r="J208" t="s">
-        <v>147</v>
-      </c>
-      <c r="K208" t="s">
-        <v>171</v>
-      </c>
       <c r="L208" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="209" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B209">
         <v>34</v>
@@ -4030,7 +4081,7 @@
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B210">
         <v>35</v>
@@ -4041,7 +4092,7 @@
     </row>
     <row r="211" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B211">
         <v>35</v>
@@ -4052,7 +4103,7 @@
     </row>
     <row r="212" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B212">
         <v>35</v>
@@ -4063,7 +4114,7 @@
     </row>
     <row r="213" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B213">
         <v>36</v>
@@ -4074,7 +4125,7 @@
     </row>
     <row r="214" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B214">
         <v>36</v>
@@ -4085,7 +4136,7 @@
     </row>
     <row r="215" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B215">
         <v>36</v>
@@ -4096,7 +4147,7 @@
     </row>
     <row r="216" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B216">
         <v>37</v>
@@ -4107,7 +4158,7 @@
     </row>
     <row r="217" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B217">
         <v>37</v>
@@ -4118,7 +4169,7 @@
     </row>
     <row r="218" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B218">
         <v>37</v>
@@ -4129,7 +4180,7 @@
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B219">
         <v>38</v>
@@ -4140,7 +4191,7 @@
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B220">
         <v>38</v>
@@ -4151,7 +4202,7 @@
     </row>
     <row r="221" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B221">
         <v>39</v>
@@ -4162,7 +4213,7 @@
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B222">
         <v>39</v>
@@ -4173,7 +4224,7 @@
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B223">
         <v>40</v>
@@ -4184,7 +4235,7 @@
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B224">
         <v>40</v>
@@ -4193,33 +4244,33 @@
         <v>1868</v>
       </c>
       <c r="D224" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E224" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F224" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G224" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I224" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J224" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K224" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L224" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="225" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B225">
         <v>41</v>
@@ -4228,33 +4279,33 @@
         <v>1868</v>
       </c>
       <c r="D225" t="s">
+        <v>168</v>
+      </c>
+      <c r="E225" t="s">
+        <v>154</v>
+      </c>
+      <c r="F225" t="s">
         <v>167</v>
       </c>
-      <c r="E225" t="s">
-        <v>153</v>
-      </c>
-      <c r="F225" t="s">
-        <v>166</v>
-      </c>
       <c r="G225" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I225" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="J225" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K225" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L225" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B226">
         <v>41</v>
@@ -4265,7 +4316,7 @@
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B227">
         <v>42</v>
@@ -4276,7 +4327,7 @@
     </row>
     <row r="228" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B228">
         <v>42</v>
@@ -4287,7 +4338,7 @@
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B229">
         <v>43</v>
@@ -4298,7 +4349,7 @@
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B230">
         <v>43</v>
@@ -4309,7 +4360,7 @@
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B231">
         <v>43</v>
@@ -4320,7 +4371,7 @@
     </row>
     <row r="232" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B232">
         <v>44</v>
@@ -4331,7 +4382,7 @@
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B233">
         <v>44</v>
@@ -4342,7 +4393,7 @@
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B234">
         <v>44</v>
@@ -4353,7 +4404,7 @@
     </row>
     <row r="235" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B235">
         <v>45</v>
@@ -4362,33 +4413,33 @@
         <v>1870</v>
       </c>
       <c r="D235" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E235" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F235" t="s">
+        <v>177</v>
+      </c>
+      <c r="G235" t="s">
+        <v>178</v>
+      </c>
+      <c r="I235" t="s">
         <v>176</v>
       </c>
-      <c r="G235" t="s">
-        <v>177</v>
-      </c>
-      <c r="I235" t="s">
-        <v>175</v>
-      </c>
       <c r="J235" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K235" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="L235" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B236">
         <v>45</v>
@@ -4399,7 +4450,7 @@
     </row>
     <row r="237" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B237">
         <v>45</v>
@@ -4410,7 +4461,7 @@
     </row>
     <row r="238" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B238">
         <v>46</v>
@@ -4421,7 +4472,7 @@
     </row>
     <row r="239" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B239">
         <v>46</v>
@@ -4432,7 +4483,7 @@
     </row>
     <row r="240" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B240">
         <v>46</v>
@@ -4443,7 +4494,7 @@
     </row>
     <row r="241" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B241">
         <v>47</v>
@@ -4454,7 +4505,7 @@
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B242">
         <v>47</v>
@@ -4465,7 +4516,7 @@
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B243">
         <v>47</v>
@@ -4476,7 +4527,7 @@
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B244">
         <v>48</v>
@@ -4487,7 +4538,7 @@
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B245">
         <v>48</v>
@@ -4498,7 +4549,7 @@
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B246">
         <v>48</v>
@@ -4509,7 +4560,7 @@
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B247">
         <v>49</v>
@@ -4518,33 +4569,33 @@
         <v>1873</v>
       </c>
       <c r="D247" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E247" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F247" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G247" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I247" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J247" t="s">
+        <v>189</v>
+      </c>
+      <c r="K247" t="s">
+        <v>190</v>
+      </c>
+      <c r="L247" t="s">
         <v>188</v>
-      </c>
-      <c r="K247" t="s">
-        <v>189</v>
-      </c>
-      <c r="L247" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B248">
         <v>49</v>
@@ -4553,33 +4604,33 @@
         <v>1873</v>
       </c>
       <c r="D248" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E248" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F248" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G248" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I248" t="s">
+        <v>194</v>
+      </c>
+      <c r="J248" t="s">
+        <v>195</v>
+      </c>
+      <c r="K248" t="s">
+        <v>196</v>
+      </c>
+      <c r="L248" t="s">
         <v>193</v>
-      </c>
-      <c r="J248" t="s">
-        <v>194</v>
-      </c>
-      <c r="K248" t="s">
-        <v>195</v>
-      </c>
-      <c r="L248" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B249">
         <v>49</v>
@@ -4588,33 +4639,33 @@
         <v>1873</v>
       </c>
       <c r="D249" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E249" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F249" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G249" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I249" t="s">
+        <v>194</v>
+      </c>
+      <c r="J249" t="s">
+        <v>195</v>
+      </c>
+      <c r="K249" t="s">
+        <v>196</v>
+      </c>
+      <c r="L249" t="s">
         <v>193</v>
-      </c>
-      <c r="J249" t="s">
-        <v>194</v>
-      </c>
-      <c r="K249" t="s">
-        <v>195</v>
-      </c>
-      <c r="L249" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B250">
         <v>50</v>
@@ -4625,7 +4676,7 @@
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B251">
         <v>50</v>
@@ -4636,7 +4687,7 @@
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B252">
         <v>51</v>
@@ -4647,7 +4698,7 @@
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B253">
         <v>51</v>
@@ -4658,13 +4709,446 @@
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B254">
         <v>51</v>
       </c>
       <c r="C254">
         <v>1873</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>198</v>
+      </c>
+      <c r="B255">
+        <v>52</v>
+      </c>
+      <c r="C255">
+        <v>1873</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>199</v>
+      </c>
+      <c r="B256">
+        <v>52</v>
+      </c>
+      <c r="C256">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="257" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>114</v>
+      </c>
+      <c r="B257">
+        <v>53</v>
+      </c>
+      <c r="C257">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="258" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>143</v>
+      </c>
+      <c r="B258">
+        <v>53</v>
+      </c>
+      <c r="C258">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="259" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>53</v>
+      </c>
+      <c r="B259">
+        <v>54</v>
+      </c>
+      <c r="C259">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="260" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>103</v>
+      </c>
+      <c r="B260">
+        <v>54</v>
+      </c>
+      <c r="C260">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="261" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>200</v>
+      </c>
+      <c r="B261">
+        <v>55</v>
+      </c>
+      <c r="C261">
+        <v>1874</v>
+      </c>
+      <c r="Q261" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="262" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>202</v>
+      </c>
+      <c r="B262">
+        <v>55</v>
+      </c>
+      <c r="C262">
+        <v>1875</v>
+      </c>
+      <c r="Q262" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="263" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>21</v>
+      </c>
+      <c r="B263">
+        <v>56</v>
+      </c>
+      <c r="C263">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="264" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>58</v>
+      </c>
+      <c r="B264">
+        <v>56</v>
+      </c>
+      <c r="C264">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="265" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>183</v>
+      </c>
+      <c r="B265">
+        <v>57</v>
+      </c>
+      <c r="C265">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="266" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>141</v>
+      </c>
+      <c r="B266">
+        <v>57</v>
+      </c>
+      <c r="C266">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="267" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>103</v>
+      </c>
+      <c r="B267">
+        <v>58</v>
+      </c>
+      <c r="C267">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="268" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>174</v>
+      </c>
+      <c r="B268">
+        <v>58</v>
+      </c>
+      <c r="C268">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="269" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>203</v>
+      </c>
+      <c r="B269">
+        <v>59</v>
+      </c>
+      <c r="C269">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="270" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>200</v>
+      </c>
+      <c r="B270">
+        <v>59</v>
+      </c>
+      <c r="C270">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="271" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>44</v>
+      </c>
+      <c r="B271">
+        <v>60</v>
+      </c>
+      <c r="C271">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="272" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>58</v>
+      </c>
+      <c r="B272">
+        <v>60</v>
+      </c>
+      <c r="C272">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="273" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>158</v>
+      </c>
+      <c r="B273">
+        <v>61</v>
+      </c>
+      <c r="C273">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="274" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>21</v>
+      </c>
+      <c r="B274">
+        <v>61</v>
+      </c>
+      <c r="C274">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>183</v>
+      </c>
+      <c r="B275">
+        <v>63</v>
+      </c>
+      <c r="C275">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>53</v>
+      </c>
+      <c r="B276">
+        <v>63</v>
+      </c>
+      <c r="C276">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>181</v>
+      </c>
+      <c r="B277">
+        <v>64</v>
+      </c>
+      <c r="C277">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>204</v>
+      </c>
+      <c r="B278">
+        <v>64</v>
+      </c>
+      <c r="C278">
+        <v>1878</v>
+      </c>
+      <c r="D278" t="s">
+        <v>184</v>
+      </c>
+      <c r="E278" t="s">
+        <v>185</v>
+      </c>
+      <c r="F278" t="s">
+        <v>177</v>
+      </c>
+      <c r="G278" t="s">
+        <v>178</v>
+      </c>
+      <c r="I278" t="s">
+        <v>206</v>
+      </c>
+      <c r="J278" t="s">
+        <v>207</v>
+      </c>
+      <c r="K278" t="s">
+        <v>149</v>
+      </c>
+      <c r="L278" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="279" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>103</v>
+      </c>
+      <c r="B279">
+        <v>65</v>
+      </c>
+      <c r="C279">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="280" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>203</v>
+      </c>
+      <c r="B280">
+        <v>65</v>
+      </c>
+      <c r="C280">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="281" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>44</v>
+      </c>
+      <c r="B281">
+        <v>66</v>
+      </c>
+      <c r="C281">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="282" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>208</v>
+      </c>
+      <c r="B282">
+        <v>66</v>
+      </c>
+      <c r="C282">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="283" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>209</v>
+      </c>
+      <c r="B283">
+        <v>67</v>
+      </c>
+      <c r="C283">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="284" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>103</v>
+      </c>
+      <c r="B284">
+        <v>67</v>
+      </c>
+      <c r="C284">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>210</v>
+      </c>
+      <c r="B285">
+        <v>68</v>
+      </c>
+      <c r="C285">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="286" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>210</v>
+      </c>
+      <c r="B286">
+        <v>68</v>
+      </c>
+      <c r="C286">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="287" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>183</v>
+      </c>
+      <c r="B287">
+        <v>69</v>
+      </c>
+      <c r="C287">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="288" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>211</v>
+      </c>
+      <c r="B288">
+        <v>69</v>
+      </c>
+      <c r="C288">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="289" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>212</v>
+      </c>
+      <c r="B289">
+        <v>70</v>
+      </c>
+      <c r="C289">
+        <v>1880</v>
+      </c>
+      <c r="D289" t="s">
+        <v>169</v>
+      </c>
+      <c r="E289" t="s">
+        <v>170</v>
+      </c>
+      <c r="F289" t="s">
+        <v>161</v>
+      </c>
+      <c r="G289" t="s">
+        <v>162</v>
+      </c>
+      <c r="I289" t="s">
+        <v>213</v>
+      </c>
+      <c r="L289" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completat indexació llibres baptismasls blancafort 1852-1895
</commit_message>
<xml_diff>
--- a/Bisbats/Catalunya/Lleida/Blancafort/Sacraments/Baptismes/Excel/Baptismes_Parroquia_Blancafort.xlsx
+++ b/Bisbats/Catalunya/Lleida/Blancafort/Sacraments/Baptismes/Excel/Baptismes_Parroquia_Blancafort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vstudio-code\repositorisArbre\DadesGenerals\Bisbats\Catalunya\Lleida\Blancafort\Sacraments\Baptismes\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71A0723-FBF3-42CF-AABE-C70E92494207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C53757-E3B2-4DC7-BEE4-39EE0132F724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="253">
   <si>
     <t>Cognoms</t>
   </si>
@@ -468,6 +468,9 @@
     <t>Gessé Gessé Clara Antonia Josepa</t>
   </si>
   <si>
+    <t>Teresa Gessé</t>
+  </si>
+  <si>
     <t>Bonaventura Gessé Medarda Farré</t>
   </si>
   <si>
@@ -718,6 +721,72 @@
   </si>
   <si>
     <t>Farré Estada</t>
+  </si>
+  <si>
+    <t>Gessé Castells</t>
+  </si>
+  <si>
+    <t>Badia Safont</t>
+  </si>
+  <si>
+    <t>05/01/1887</t>
+  </si>
+  <si>
+    <t>Gessé Gessé Antoni  Josep</t>
+  </si>
+  <si>
+    <t>04/01/1887</t>
+  </si>
+  <si>
+    <t>Antoni Gessé Santamaria</t>
+  </si>
+  <si>
+    <t>Maria Gessé Badia</t>
+  </si>
+  <si>
+    <t>Gessé Pijoan</t>
+  </si>
+  <si>
+    <t>12/03/1887</t>
+  </si>
+  <si>
+    <t>Gessé Gessé Antoni Josep</t>
+  </si>
+  <si>
+    <t>11/03/1887</t>
+  </si>
+  <si>
+    <t>Blas Gessé i Rosa Santamaria</t>
+  </si>
+  <si>
+    <t>Francisco Gessé i Raimunda Badia</t>
+  </si>
+  <si>
+    <t>Pere Castells</t>
+  </si>
+  <si>
+    <t>Melchora Garcia</t>
+  </si>
+  <si>
+    <t>Camarasa Castells</t>
+  </si>
+  <si>
+    <t>Gessé Piguan</t>
+  </si>
+  <si>
+    <t>Gessé Pena</t>
+  </si>
+  <si>
+    <t>Gessé Miranda Maria Teresa</t>
+  </si>
+  <si>
+    <t>14/07/1895</t>
+  </si>
+  <si>
+    <t>13/07/1895</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medardo Miranda </t>
   </si>
 </sst>
 </file>
@@ -1052,11 +1121,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q307"/>
+  <dimension ref="A1:Q350"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A283" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B308" sqref="B308"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A335" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O364" sqref="O364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3234,6 +3303,9 @@
       <c r="C132">
         <v>1852</v>
       </c>
+      <c r="P132" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
@@ -3245,6 +3317,9 @@
       <c r="C133">
         <v>1852</v>
       </c>
+      <c r="P133" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
@@ -3256,6 +3331,9 @@
       <c r="C134">
         <v>1852</v>
       </c>
+      <c r="P134" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
@@ -3267,6 +3345,9 @@
       <c r="C135">
         <v>1852</v>
       </c>
+      <c r="P135" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
@@ -3278,6 +3359,9 @@
       <c r="C136">
         <v>1852</v>
       </c>
+      <c r="P136" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
@@ -3289,6 +3373,9 @@
       <c r="C137">
         <v>1852</v>
       </c>
+      <c r="P137" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
@@ -3297,6 +3384,9 @@
       <c r="B138" s="4" t="s">
         <v>120</v>
       </c>
+      <c r="P138" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
@@ -3308,6 +3398,9 @@
       <c r="C139">
         <v>1852</v>
       </c>
+      <c r="P139" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
@@ -3319,6 +3412,9 @@
       <c r="C140">
         <v>1853</v>
       </c>
+      <c r="P140" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
@@ -3330,6 +3426,9 @@
       <c r="C141">
         <v>1853</v>
       </c>
+      <c r="P141" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
@@ -3341,6 +3440,9 @@
       <c r="C142">
         <v>1853</v>
       </c>
+      <c r="P142" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
@@ -3352,6 +3454,9 @@
       <c r="C143">
         <v>1853</v>
       </c>
+      <c r="P143" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
@@ -3363,8 +3468,11 @@
       <c r="C144">
         <v>1853</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P144" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>55</v>
       </c>
@@ -3374,8 +3482,11 @@
       <c r="C145">
         <v>1853</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P145" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>117</v>
       </c>
@@ -3385,8 +3496,11 @@
       <c r="C146">
         <v>1854</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P146" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>125</v>
       </c>
@@ -3396,8 +3510,11 @@
       <c r="C147">
         <v>1854</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P147" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>126</v>
       </c>
@@ -3407,8 +3524,11 @@
       <c r="C148">
         <v>1854</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P148" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>127</v>
       </c>
@@ -3418,8 +3538,11 @@
       <c r="C149">
         <v>1854</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P149" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>128</v>
       </c>
@@ -3429,8 +3552,11 @@
       <c r="C150">
         <v>1854</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P150" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>103</v>
       </c>
@@ -3440,8 +3566,11 @@
       <c r="C151">
         <v>1854</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P151" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>116</v>
       </c>
@@ -3451,8 +3580,11 @@
       <c r="C152">
         <v>1854</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P152" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>129</v>
       </c>
@@ -3462,8 +3594,11 @@
       <c r="C153">
         <v>1855</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P153" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>130</v>
       </c>
@@ -3473,8 +3608,11 @@
       <c r="C154">
         <v>1855</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P154" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>131</v>
       </c>
@@ -3484,8 +3622,11 @@
       <c r="C155">
         <v>1855</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P155" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>121</v>
       </c>
@@ -3495,8 +3636,11 @@
       <c r="C156">
         <v>1855</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P156" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>122</v>
       </c>
@@ -3506,8 +3650,11 @@
       <c r="C157">
         <v>1855</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P157" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>55</v>
       </c>
@@ -3517,8 +3664,11 @@
       <c r="C158">
         <v>1856</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P158" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>128</v>
       </c>
@@ -3528,8 +3678,11 @@
       <c r="C159">
         <v>1856</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P159" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>114</v>
       </c>
@@ -3539,8 +3692,11 @@
       <c r="C160">
         <v>1856</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P160" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>103</v>
       </c>
@@ -3550,8 +3706,11 @@
       <c r="C161">
         <v>1856</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P161" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>132</v>
       </c>
@@ -3561,8 +3720,11 @@
       <c r="C162">
         <v>1857</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P162" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>116</v>
       </c>
@@ -3572,8 +3734,11 @@
       <c r="C163">
         <v>1857</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P163" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>133</v>
       </c>
@@ -3583,8 +3748,11 @@
       <c r="C164">
         <v>1857</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P164" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>134</v>
       </c>
@@ -3594,8 +3762,11 @@
       <c r="C165">
         <v>1857</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P165" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>128</v>
       </c>
@@ -3605,8 +3776,11 @@
       <c r="C166">
         <v>1858</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P166" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>135</v>
       </c>
@@ -3616,8 +3790,11 @@
       <c r="C167">
         <v>1858</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P167" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>131</v>
       </c>
@@ -3627,8 +3804,11 @@
       <c r="C168">
         <v>1858</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P168" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>136</v>
       </c>
@@ -3638,8 +3818,11 @@
       <c r="C169">
         <v>1858</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P169" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>58</v>
       </c>
@@ -3649,8 +3832,11 @@
       <c r="C170">
         <v>1858</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P170" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>55</v>
       </c>
@@ -3660,8 +3846,11 @@
       <c r="C171">
         <v>1858</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P171" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>122</v>
       </c>
@@ -3671,8 +3860,11 @@
       <c r="C172">
         <v>1858</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P172" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>116</v>
       </c>
@@ -3682,8 +3874,11 @@
       <c r="C173">
         <v>1859</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P173" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>133</v>
       </c>
@@ -3693,8 +3888,11 @@
       <c r="C174">
         <v>1860</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P174" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>137</v>
       </c>
@@ -3704,8 +3902,11 @@
       <c r="C175">
         <v>1860</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P175" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>114</v>
       </c>
@@ -3715,8 +3916,11 @@
       <c r="C176">
         <v>1860</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P176" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="177" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>55</v>
       </c>
@@ -3726,8 +3930,11 @@
       <c r="C177">
         <v>1860</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P177" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="178" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>138</v>
       </c>
@@ -3737,8 +3944,11 @@
       <c r="C178">
         <v>1860</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P178" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>139</v>
       </c>
@@ -3748,8 +3958,11 @@
       <c r="C179">
         <v>1860</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P179" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="180" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>123</v>
       </c>
@@ -3759,8 +3972,11 @@
       <c r="C180">
         <v>1860</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P180" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="181" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>132</v>
       </c>
@@ -3770,8 +3986,11 @@
       <c r="C181">
         <v>1860</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P181" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="182" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>140</v>
       </c>
@@ -3781,8 +4000,11 @@
       <c r="C182">
         <v>1861</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P182" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="183" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>58</v>
       </c>
@@ -3792,8 +4014,11 @@
       <c r="C183">
         <v>1861</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P183" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>141</v>
       </c>
@@ -3803,8 +4028,11 @@
       <c r="C184">
         <v>1861</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P184" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="185" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>142</v>
       </c>
@@ -3814,8 +4042,11 @@
       <c r="C185">
         <v>1861</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P185" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="186" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>55</v>
       </c>
@@ -3825,8 +4056,11 @@
       <c r="C186">
         <v>1861</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P186" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="187" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>114</v>
       </c>
@@ -3836,8 +4070,11 @@
       <c r="C187">
         <v>1861</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P187" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="188" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>114</v>
       </c>
@@ -3847,8 +4084,11 @@
       <c r="C188">
         <v>1862</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P188" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="189" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>122</v>
       </c>
@@ -3858,8 +4098,11 @@
       <c r="C189">
         <v>1862</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P189" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="190" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>143</v>
       </c>
@@ -3869,8 +4112,11 @@
       <c r="C190">
         <v>1862</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P190" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="191" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>116</v>
       </c>
@@ -3880,8 +4126,11 @@
       <c r="C191">
         <v>1862</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P191" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="192" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>128</v>
       </c>
@@ -3891,8 +4140,11 @@
       <c r="C192">
         <v>1863</v>
       </c>
-    </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P192" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="193" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>114</v>
       </c>
@@ -3902,8 +4154,11 @@
       <c r="C193">
         <v>1863</v>
       </c>
-    </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P193" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="194" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>133</v>
       </c>
@@ -3913,8 +4168,11 @@
       <c r="C194">
         <v>1863</v>
       </c>
-    </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P194" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="195" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>139</v>
       </c>
@@ -3924,8 +4182,11 @@
       <c r="C195">
         <v>1863</v>
       </c>
-    </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P195" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="196" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>145</v>
       </c>
@@ -3939,28 +4200,31 @@
         <v>75</v>
       </c>
       <c r="E196" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F196" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G196" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I196" t="s">
         <v>144</v>
       </c>
       <c r="J196" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K196" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L196" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P196" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="197" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>141</v>
       </c>
@@ -3970,8 +4234,11 @@
       <c r="C197">
         <v>1863</v>
       </c>
-    </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P197" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="198" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>114</v>
       </c>
@@ -3981,10 +4248,13 @@
       <c r="C198">
         <v>1863</v>
       </c>
-    </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P198" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="199" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B199">
         <v>31</v>
@@ -3992,8 +4262,11 @@
       <c r="C199">
         <v>1863</v>
       </c>
-    </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P199" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="200" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>135</v>
       </c>
@@ -4003,8 +4276,11 @@
       <c r="C200">
         <v>1864</v>
       </c>
-    </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P200" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="201" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>55</v>
       </c>
@@ -4014,10 +4290,13 @@
       <c r="C201">
         <v>1864</v>
       </c>
-    </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P201" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B202">
         <v>32</v>
@@ -4025,8 +4304,11 @@
       <c r="C202">
         <v>1864</v>
       </c>
-    </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P202" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="203" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>143</v>
       </c>
@@ -4036,8 +4318,11 @@
       <c r="C203">
         <v>1864</v>
       </c>
-    </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P203" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="204" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>123</v>
       </c>
@@ -4047,8 +4332,11 @@
       <c r="C204">
         <v>1864</v>
       </c>
-    </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P204" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>139</v>
       </c>
@@ -4058,8 +4346,11 @@
       <c r="C205">
         <v>1865</v>
       </c>
-    </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P205" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="206" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>114</v>
       </c>
@@ -4069,8 +4360,11 @@
       <c r="C206">
         <v>1865</v>
       </c>
-    </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P206" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>128</v>
       </c>
@@ -4080,10 +4374,13 @@
       <c r="C207">
         <v>1865</v>
       </c>
-    </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P207" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B208">
         <v>34</v>
@@ -4092,31 +4389,34 @@
         <v>1866</v>
       </c>
       <c r="D208" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E208" t="s">
+        <v>174</v>
+      </c>
+      <c r="F208" t="s">
+        <v>172</v>
+      </c>
+      <c r="G208" t="s">
+        <v>148</v>
+      </c>
+      <c r="I208" t="s">
+        <v>153</v>
+      </c>
+      <c r="J208" t="s">
+        <v>149</v>
+      </c>
+      <c r="K208" t="s">
         <v>173</v>
       </c>
-      <c r="F208" t="s">
-        <v>171</v>
-      </c>
-      <c r="G208" t="s">
-        <v>147</v>
-      </c>
-      <c r="I208" t="s">
-        <v>152</v>
-      </c>
-      <c r="J208" t="s">
-        <v>148</v>
-      </c>
-      <c r="K208" t="s">
-        <v>172</v>
-      </c>
       <c r="L208" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="P208" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="209" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>116</v>
       </c>
@@ -4126,8 +4426,11 @@
       <c r="C209">
         <v>1866</v>
       </c>
-    </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P209" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="210" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>141</v>
       </c>
@@ -4137,10 +4440,13 @@
       <c r="C210">
         <v>1866</v>
       </c>
-    </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P210" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="211" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B211">
         <v>35</v>
@@ -4148,8 +4454,11 @@
       <c r="C211">
         <v>1866</v>
       </c>
-    </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P211" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="212" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>114</v>
       </c>
@@ -4159,8 +4468,11 @@
       <c r="C212">
         <v>1866</v>
       </c>
-    </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P212" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="213" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>53</v>
       </c>
@@ -4170,10 +4482,13 @@
       <c r="C213">
         <v>1866</v>
       </c>
-    </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P213" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="214" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B214">
         <v>36</v>
@@ -4181,8 +4496,11 @@
       <c r="C214">
         <v>1866</v>
       </c>
-    </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P214" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="215" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>137</v>
       </c>
@@ -4192,10 +4510,13 @@
       <c r="C215">
         <v>1866</v>
       </c>
-    </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P215" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="216" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B216">
         <v>37</v>
@@ -4203,8 +4524,11 @@
       <c r="C216">
         <v>1867</v>
       </c>
-    </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P216" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="217" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>143</v>
       </c>
@@ -4214,8 +4538,11 @@
       <c r="C217">
         <v>1867</v>
       </c>
-    </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P217" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="218" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>122</v>
       </c>
@@ -4225,10 +4552,13 @@
       <c r="C218">
         <v>1867</v>
       </c>
-    </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P218" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="219" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B219">
         <v>38</v>
@@ -4236,8 +4566,11 @@
       <c r="C219">
         <v>1868</v>
       </c>
-    </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P219" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="220" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>114</v>
       </c>
@@ -4247,8 +4580,11 @@
       <c r="C220">
         <v>1868</v>
       </c>
-    </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P220" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="221" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>103</v>
       </c>
@@ -4258,8 +4594,11 @@
       <c r="C221">
         <v>1868</v>
       </c>
-    </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P221" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="222" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>141</v>
       </c>
@@ -4269,8 +4608,11 @@
       <c r="C222">
         <v>1868</v>
       </c>
-    </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P222" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="223" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>103</v>
       </c>
@@ -4280,10 +4622,13 @@
       <c r="C223">
         <v>1868</v>
       </c>
-    </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P223" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="224" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B224">
         <v>40</v>
@@ -4292,33 +4637,36 @@
         <v>1868</v>
       </c>
       <c r="D224" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E224" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F224" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G224" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I224" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="J224" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K224" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="L224" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="P224" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="225" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B225">
         <v>41</v>
@@ -4327,31 +4675,34 @@
         <v>1868</v>
       </c>
       <c r="D225" t="s">
+        <v>169</v>
+      </c>
+      <c r="E225" t="s">
+        <v>155</v>
+      </c>
+      <c r="F225" t="s">
         <v>168</v>
       </c>
-      <c r="E225" t="s">
-        <v>154</v>
-      </c>
-      <c r="F225" t="s">
-        <v>167</v>
-      </c>
       <c r="G225" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I225" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J225" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K225" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L225" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="P225" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="226" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>116</v>
       </c>
@@ -4361,8 +4712,11 @@
       <c r="C226">
         <v>1869</v>
       </c>
-    </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P226" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="227" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>114</v>
       </c>
@@ -4372,8 +4726,11 @@
       <c r="C227">
         <v>1869</v>
       </c>
-    </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P227" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="228" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>143</v>
       </c>
@@ -4383,10 +4740,13 @@
       <c r="C228">
         <v>1869</v>
       </c>
-    </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P228" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="229" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B229">
         <v>43</v>
@@ -4394,8 +4754,11 @@
       <c r="C229">
         <v>1869</v>
       </c>
-    </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P229" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="230" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>128</v>
       </c>
@@ -4405,10 +4768,13 @@
       <c r="C230">
         <v>1869</v>
       </c>
-    </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P230" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="231" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B231">
         <v>43</v>
@@ -4416,8 +4782,11 @@
       <c r="C231">
         <v>1869</v>
       </c>
-    </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P231" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="232" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>139</v>
       </c>
@@ -4427,8 +4796,11 @@
       <c r="C232">
         <v>1869</v>
       </c>
-    </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P232" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="233" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>114</v>
       </c>
@@ -4438,8 +4810,11 @@
       <c r="C233">
         <v>1870</v>
       </c>
-    </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P233" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="234" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>53</v>
       </c>
@@ -4449,10 +4824,13 @@
       <c r="C234">
         <v>1870</v>
       </c>
-    </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P234" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="235" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B235">
         <v>45</v>
@@ -4461,33 +4839,36 @@
         <v>1870</v>
       </c>
       <c r="D235" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E235" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F235" t="s">
+        <v>178</v>
+      </c>
+      <c r="G235" t="s">
+        <v>179</v>
+      </c>
+      <c r="I235" t="s">
         <v>177</v>
       </c>
-      <c r="G235" t="s">
-        <v>178</v>
-      </c>
-      <c r="I235" t="s">
-        <v>176</v>
-      </c>
       <c r="J235" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K235" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="L235" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="P235" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="236" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B236">
         <v>45</v>
@@ -4495,10 +4876,13 @@
       <c r="C236">
         <v>1870</v>
       </c>
-    </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P236" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="237" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B237">
         <v>45</v>
@@ -4506,8 +4890,11 @@
       <c r="C237">
         <v>1870</v>
       </c>
-    </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P237" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="238" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>133</v>
       </c>
@@ -4517,10 +4904,13 @@
       <c r="C238">
         <v>1871</v>
       </c>
-    </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P238" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="239" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B239">
         <v>46</v>
@@ -4528,8 +4918,11 @@
       <c r="C239">
         <v>1871</v>
       </c>
-    </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P239" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="240" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>114</v>
       </c>
@@ -4539,10 +4932,13 @@
       <c r="C240">
         <v>1871</v>
       </c>
-    </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P240" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="241" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B241">
         <v>47</v>
@@ -4550,8 +4946,11 @@
       <c r="C241">
         <v>1871</v>
       </c>
-    </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P241" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="242" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>141</v>
       </c>
@@ -4561,8 +4960,11 @@
       <c r="C242">
         <v>1871</v>
       </c>
-    </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P242" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="243" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>44</v>
       </c>
@@ -4572,8 +4974,11 @@
       <c r="C243">
         <v>1872</v>
       </c>
-    </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P243" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="244" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>143</v>
       </c>
@@ -4583,8 +4988,11 @@
       <c r="C244">
         <v>1872</v>
       </c>
-    </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P244" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="245" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>103</v>
       </c>
@@ -4594,10 +5002,13 @@
       <c r="C245">
         <v>1872</v>
       </c>
-    </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P245" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="246" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B246">
         <v>48</v>
@@ -4605,10 +5016,13 @@
       <c r="C246">
         <v>1873</v>
       </c>
-    </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P246" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="247" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B247">
         <v>49</v>
@@ -4617,33 +5031,36 @@
         <v>1873</v>
       </c>
       <c r="D247" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E247" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F247" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G247" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I247" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="J247" t="s">
+        <v>190</v>
+      </c>
+      <c r="K247" t="s">
+        <v>191</v>
+      </c>
+      <c r="L247" t="s">
         <v>189</v>
       </c>
-      <c r="K247" t="s">
-        <v>190</v>
-      </c>
-      <c r="L247" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P247" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="248" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B248">
         <v>49</v>
@@ -4652,33 +5069,36 @@
         <v>1873</v>
       </c>
       <c r="D248" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E248" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F248" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G248" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I248" t="s">
+        <v>195</v>
+      </c>
+      <c r="J248" t="s">
+        <v>196</v>
+      </c>
+      <c r="K248" t="s">
+        <v>197</v>
+      </c>
+      <c r="L248" t="s">
         <v>194</v>
       </c>
-      <c r="J248" t="s">
-        <v>195</v>
-      </c>
-      <c r="K248" t="s">
-        <v>196</v>
-      </c>
-      <c r="L248" t="s">
+      <c r="P248" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="249" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
         <v>193</v>
-      </c>
-    </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
-        <v>192</v>
       </c>
       <c r="B249">
         <v>49</v>
@@ -4687,31 +5107,34 @@
         <v>1873</v>
       </c>
       <c r="D249" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E249" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F249" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G249" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I249" t="s">
+        <v>195</v>
+      </c>
+      <c r="J249" t="s">
+        <v>196</v>
+      </c>
+      <c r="K249" t="s">
+        <v>197</v>
+      </c>
+      <c r="L249" t="s">
         <v>194</v>
       </c>
-      <c r="J249" t="s">
-        <v>195</v>
-      </c>
-      <c r="K249" t="s">
-        <v>196</v>
-      </c>
-      <c r="L249" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P249" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="250" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>56</v>
       </c>
@@ -4721,10 +5144,13 @@
       <c r="C250">
         <v>1873</v>
       </c>
-    </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P250" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="251" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B251">
         <v>50</v>
@@ -4732,10 +5158,13 @@
       <c r="C251">
         <v>1873</v>
       </c>
-    </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P251" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="252" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B252">
         <v>51</v>
@@ -4743,8 +5172,11 @@
       <c r="C252">
         <v>1873</v>
       </c>
-    </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P252" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="253" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>141</v>
       </c>
@@ -4754,10 +5186,13 @@
       <c r="C253">
         <v>1873</v>
       </c>
-    </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P253" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="254" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B254">
         <v>51</v>
@@ -4765,10 +5200,13 @@
       <c r="C254">
         <v>1873</v>
       </c>
-    </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P254" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="255" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B255">
         <v>52</v>
@@ -4776,16 +5214,22 @@
       <c r="C255">
         <v>1873</v>
       </c>
-    </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P255" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="256" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B256">
         <v>52</v>
       </c>
       <c r="C256">
         <v>1874</v>
+      </c>
+      <c r="P256" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="257" spans="1:17" x14ac:dyDescent="0.25">
@@ -4798,6 +5242,9 @@
       <c r="C257">
         <v>1874</v>
       </c>
+      <c r="P257" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="258" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
@@ -4809,6 +5256,9 @@
       <c r="C258">
         <v>1874</v>
       </c>
+      <c r="P258" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="259" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
@@ -4820,6 +5270,9 @@
       <c r="C259">
         <v>1874</v>
       </c>
+      <c r="P259" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="260" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
@@ -4831,10 +5284,13 @@
       <c r="C260">
         <v>1874</v>
       </c>
+      <c r="P260" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="261" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B261">
         <v>55</v>
@@ -4842,13 +5298,16 @@
       <c r="C261">
         <v>1874</v>
       </c>
+      <c r="P261" t="s">
+        <v>113</v>
+      </c>
       <c r="Q261" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="262" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B262">
         <v>55</v>
@@ -4856,8 +5315,11 @@
       <c r="C262">
         <v>1875</v>
       </c>
+      <c r="P262" t="s">
+        <v>113</v>
+      </c>
       <c r="Q262" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="263" spans="1:17" x14ac:dyDescent="0.25">
@@ -4870,6 +5332,9 @@
       <c r="C263">
         <v>1875</v>
       </c>
+      <c r="P263" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="264" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
@@ -4881,16 +5346,22 @@
       <c r="C264">
         <v>1875</v>
       </c>
+      <c r="P264" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="265" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B265">
         <v>57</v>
       </c>
       <c r="C265">
         <v>1876</v>
+      </c>
+      <c r="P265" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="266" spans="1:17" x14ac:dyDescent="0.25">
@@ -4903,6 +5374,9 @@
       <c r="C266">
         <v>1876</v>
       </c>
+      <c r="P266" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="267" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
@@ -4914,10 +5388,13 @@
       <c r="C267">
         <v>1876</v>
       </c>
+      <c r="P267" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="268" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B268">
         <v>58</v>
@@ -4925,10 +5402,13 @@
       <c r="C268">
         <v>1876</v>
       </c>
+      <c r="P268" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="269" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B269">
         <v>59</v>
@@ -4936,16 +5416,22 @@
       <c r="C269">
         <v>1876</v>
       </c>
+      <c r="P269" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="270" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B270">
         <v>59</v>
       </c>
       <c r="C270">
         <v>1877</v>
+      </c>
+      <c r="P270" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="271" spans="1:17" x14ac:dyDescent="0.25">
@@ -4958,6 +5444,9 @@
       <c r="C271">
         <v>1877</v>
       </c>
+      <c r="P271" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="272" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
@@ -4969,10 +5458,13 @@
       <c r="C272">
         <v>1877</v>
       </c>
-    </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P272" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="273" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B273">
         <v>61</v>
@@ -4980,8 +5472,11 @@
       <c r="C273">
         <v>1877</v>
       </c>
-    </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P273" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="274" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>21</v>
       </c>
@@ -4991,10 +5486,13 @@
       <c r="C274">
         <v>1877</v>
       </c>
-    </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P274" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="275" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B275">
         <v>63</v>
@@ -5002,8 +5500,11 @@
       <c r="C275">
         <v>1877</v>
       </c>
-    </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P275" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="276" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>53</v>
       </c>
@@ -5013,10 +5514,13 @@
       <c r="C276">
         <v>1877</v>
       </c>
-    </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P276" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="277" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B277">
         <v>64</v>
@@ -5024,10 +5528,13 @@
       <c r="C277">
         <v>1878</v>
       </c>
-    </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P277" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="278" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B278">
         <v>64</v>
@@ -5036,31 +5543,34 @@
         <v>1878</v>
       </c>
       <c r="D278" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E278" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F278" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G278" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I278" t="s">
+        <v>207</v>
+      </c>
+      <c r="J278" t="s">
+        <v>208</v>
+      </c>
+      <c r="K278" t="s">
+        <v>150</v>
+      </c>
+      <c r="L278" t="s">
         <v>206</v>
       </c>
-      <c r="J278" t="s">
-        <v>207</v>
-      </c>
-      <c r="K278" t="s">
-        <v>149</v>
-      </c>
-      <c r="L278" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P278" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="279" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>103</v>
       </c>
@@ -5070,10 +5580,13 @@
       <c r="C279">
         <v>1878</v>
       </c>
-    </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P279" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="280" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B280">
         <v>65</v>
@@ -5081,8 +5594,11 @@
       <c r="C280">
         <v>1878</v>
       </c>
-    </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P280" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="281" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>44</v>
       </c>
@@ -5092,10 +5608,13 @@
       <c r="C281">
         <v>1879</v>
       </c>
-    </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P281" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="282" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B282">
         <v>66</v>
@@ -5103,10 +5622,13 @@
       <c r="C282">
         <v>1879</v>
       </c>
-    </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P282" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="283" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B283">
         <v>67</v>
@@ -5114,8 +5636,11 @@
       <c r="C283">
         <v>1879</v>
       </c>
-    </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P283" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="284" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>103</v>
       </c>
@@ -5125,10 +5650,13 @@
       <c r="C284">
         <v>1880</v>
       </c>
-    </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P284" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="285" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B285">
         <v>68</v>
@@ -5136,10 +5664,13 @@
       <c r="C285">
         <v>1880</v>
       </c>
-    </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P285" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="286" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B286">
         <v>68</v>
@@ -5147,10 +5678,13 @@
       <c r="C286">
         <v>1880</v>
       </c>
-    </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P286" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="287" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B287">
         <v>69</v>
@@ -5158,10 +5692,13 @@
       <c r="C287">
         <v>1880</v>
       </c>
-    </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P287" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="288" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B288">
         <v>69</v>
@@ -5169,10 +5706,13 @@
       <c r="C288">
         <v>1880</v>
       </c>
+      <c r="P288" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="289" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B289">
         <v>70</v>
@@ -5181,33 +5721,36 @@
         <v>1880</v>
       </c>
       <c r="D289" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E289" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F289" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G289" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I289" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="J289" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K289" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="L289" t="s">
-        <v>213</v>
+        <v>214</v>
+      </c>
+      <c r="P289" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="290" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B290">
         <v>71</v>
@@ -5216,39 +5759,45 @@
         <v>1880</v>
       </c>
       <c r="D290" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E290" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F290" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G290" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I290" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="J290" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K290" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="L290" t="s">
-        <v>213</v>
+        <v>214</v>
+      </c>
+      <c r="P290" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="291" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B291">
         <v>72</v>
       </c>
       <c r="C291">
         <v>1881</v>
+      </c>
+      <c r="P291" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="292" spans="1:17" x14ac:dyDescent="0.25">
@@ -5261,10 +5810,13 @@
       <c r="C292">
         <v>1881</v>
       </c>
+      <c r="P292" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="293" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B293">
         <v>73</v>
@@ -5273,28 +5825,31 @@
         <v>1881</v>
       </c>
       <c r="D293" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E293" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F293" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G293" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I293" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J293" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="K293" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L293" t="s">
-        <v>218</v>
+        <v>219</v>
+      </c>
+      <c r="P293" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="294" spans="1:17" x14ac:dyDescent="0.25">
@@ -5307,13 +5862,16 @@
       <c r="C294">
         <v>1881</v>
       </c>
+      <c r="P294" t="s">
+        <v>113</v>
+      </c>
       <c r="Q294" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="295" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B295">
         <v>74</v>
@@ -5321,16 +5879,22 @@
       <c r="C295">
         <v>1882</v>
       </c>
+      <c r="P295" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="296" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B296">
         <v>75</v>
       </c>
       <c r="C296">
         <v>1882</v>
+      </c>
+      <c r="P296" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="297" spans="1:17" x14ac:dyDescent="0.25">
@@ -5343,10 +5907,13 @@
       <c r="C297">
         <v>1882</v>
       </c>
+      <c r="P297" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="298" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B298">
         <v>76</v>
@@ -5354,10 +5921,13 @@
       <c r="C298">
         <v>1883</v>
       </c>
+      <c r="P298" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="299" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B299">
         <v>76</v>
@@ -5365,16 +5935,22 @@
       <c r="C299">
         <v>1883</v>
       </c>
+      <c r="P299" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="300" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B300">
         <v>77</v>
       </c>
       <c r="C300">
         <v>1884</v>
+      </c>
+      <c r="P300" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="301" spans="1:17" x14ac:dyDescent="0.25">
@@ -5387,16 +5963,22 @@
       <c r="C301">
         <v>1884</v>
       </c>
+      <c r="P301" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="302" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B302">
         <v>78</v>
       </c>
       <c r="C302">
         <v>1884</v>
+      </c>
+      <c r="P302" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="303" spans="1:17" x14ac:dyDescent="0.25">
@@ -5409,10 +5991,13 @@
       <c r="C303">
         <v>1884</v>
       </c>
+      <c r="P303" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="304" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B304">
         <v>79</v>
@@ -5420,10 +6005,13 @@
       <c r="C304">
         <v>1885</v>
       </c>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P304" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="305" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B305">
         <v>79</v>
@@ -5431,10 +6019,13 @@
       <c r="C305">
         <v>1885</v>
       </c>
-    </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P305" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="306" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B306">
         <v>80</v>
@@ -5442,16 +6033,693 @@
       <c r="C306">
         <v>1866</v>
       </c>
-    </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P306" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="307" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B307">
         <v>80</v>
       </c>
       <c r="C307">
         <v>1866</v>
+      </c>
+      <c r="P307" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="308" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>231</v>
+      </c>
+      <c r="B308">
+        <v>81</v>
+      </c>
+      <c r="C308">
+        <v>1866</v>
+      </c>
+      <c r="P308" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="309" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>152</v>
+      </c>
+      <c r="B309">
+        <v>81</v>
+      </c>
+      <c r="C309">
+        <v>1866</v>
+      </c>
+      <c r="P309" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="310" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>212</v>
+      </c>
+      <c r="B310">
+        <v>81</v>
+      </c>
+      <c r="C310">
+        <v>1866</v>
+      </c>
+      <c r="P310" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="311" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>218</v>
+      </c>
+      <c r="B311">
+        <v>82</v>
+      </c>
+      <c r="C311">
+        <v>1866</v>
+      </c>
+      <c r="P311" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="312" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>210</v>
+      </c>
+      <c r="B312">
+        <v>82</v>
+      </c>
+      <c r="C312">
+        <v>1866</v>
+      </c>
+      <c r="P312" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="313" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>232</v>
+      </c>
+      <c r="B313">
+        <v>83</v>
+      </c>
+      <c r="C313">
+        <v>1866</v>
+      </c>
+      <c r="P313" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="314" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>234</v>
+      </c>
+      <c r="B314">
+        <v>83</v>
+      </c>
+      <c r="C314">
+        <v>1867</v>
+      </c>
+      <c r="D314" t="s">
+        <v>185</v>
+      </c>
+      <c r="E314" t="s">
+        <v>186</v>
+      </c>
+      <c r="F314" t="s">
+        <v>178</v>
+      </c>
+      <c r="G314" t="s">
+        <v>179</v>
+      </c>
+      <c r="I314" t="s">
+        <v>235</v>
+      </c>
+      <c r="J314" t="s">
+        <v>236</v>
+      </c>
+      <c r="K314" t="s">
+        <v>237</v>
+      </c>
+      <c r="L314" t="s">
+        <v>233</v>
+      </c>
+      <c r="P314" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="315" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>238</v>
+      </c>
+      <c r="B315">
+        <v>83</v>
+      </c>
+      <c r="C315">
+        <v>1867</v>
+      </c>
+      <c r="P315" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="316" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>240</v>
+      </c>
+      <c r="B316">
+        <v>84</v>
+      </c>
+      <c r="C316">
+        <v>1887</v>
+      </c>
+      <c r="D316" t="s">
+        <v>236</v>
+      </c>
+      <c r="E316" t="s">
+        <v>237</v>
+      </c>
+      <c r="F316" t="s">
+        <v>242</v>
+      </c>
+      <c r="G316" t="s">
+        <v>243</v>
+      </c>
+      <c r="I316" t="s">
+        <v>241</v>
+      </c>
+      <c r="J316" t="s">
+        <v>244</v>
+      </c>
+      <c r="K316" t="s">
+        <v>245</v>
+      </c>
+      <c r="L316" t="s">
+        <v>239</v>
+      </c>
+      <c r="P316" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="317" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>184</v>
+      </c>
+      <c r="B317">
+        <v>84</v>
+      </c>
+      <c r="C317">
+        <v>1887</v>
+      </c>
+      <c r="P317" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="318" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>175</v>
+      </c>
+      <c r="B318">
+        <v>85</v>
+      </c>
+      <c r="C318">
+        <v>1887</v>
+      </c>
+      <c r="P318" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="319" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>57</v>
+      </c>
+      <c r="B319">
+        <v>85</v>
+      </c>
+      <c r="C319">
+        <v>1887</v>
+      </c>
+      <c r="P319" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="320" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>21</v>
+      </c>
+      <c r="B320">
+        <v>86</v>
+      </c>
+      <c r="C320">
+        <v>1887</v>
+      </c>
+      <c r="P320" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="321" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>103</v>
+      </c>
+      <c r="B321">
+        <v>87</v>
+      </c>
+      <c r="C321">
+        <v>1888</v>
+      </c>
+      <c r="P321" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="322" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>59</v>
+      </c>
+      <c r="B322">
+        <v>88</v>
+      </c>
+      <c r="C322">
+        <v>1888</v>
+      </c>
+      <c r="P322" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="323" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>230</v>
+      </c>
+      <c r="B323">
+        <v>88</v>
+      </c>
+      <c r="C323">
+        <v>1889</v>
+      </c>
+      <c r="P323" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="324" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>246</v>
+      </c>
+      <c r="B324">
+        <v>89</v>
+      </c>
+      <c r="C324">
+        <v>1889</v>
+      </c>
+      <c r="P324" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="325" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>231</v>
+      </c>
+      <c r="B325">
+        <v>89</v>
+      </c>
+      <c r="C325">
+        <v>1889</v>
+      </c>
+      <c r="P325" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="326" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>64</v>
+      </c>
+      <c r="B326">
+        <v>90</v>
+      </c>
+      <c r="C326">
+        <v>1889</v>
+      </c>
+      <c r="P326" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="327" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>212</v>
+      </c>
+      <c r="B327">
+        <v>90</v>
+      </c>
+      <c r="C327">
+        <v>1889</v>
+      </c>
+      <c r="P327" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="328" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>247</v>
+      </c>
+      <c r="B328">
+        <v>91</v>
+      </c>
+      <c r="C328">
+        <v>1890</v>
+      </c>
+      <c r="P328" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="329" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>184</v>
+      </c>
+      <c r="B329">
+        <v>91</v>
+      </c>
+      <c r="C329">
+        <v>1890</v>
+      </c>
+      <c r="P329" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="330" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>103</v>
+      </c>
+      <c r="B330">
+        <v>92</v>
+      </c>
+      <c r="C330">
+        <v>1890</v>
+      </c>
+      <c r="P330" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="331" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>246</v>
+      </c>
+      <c r="B331">
+        <v>93</v>
+      </c>
+      <c r="C331">
+        <v>1891</v>
+      </c>
+      <c r="P331" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="332" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>55</v>
+      </c>
+      <c r="B332">
+        <v>93</v>
+      </c>
+      <c r="C332">
+        <v>1892</v>
+      </c>
+      <c r="P332" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="333" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>227</v>
+      </c>
+      <c r="B333">
+        <v>94</v>
+      </c>
+      <c r="C333">
+        <v>1892</v>
+      </c>
+      <c r="P333" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="334" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>212</v>
+      </c>
+      <c r="B334">
+        <v>94</v>
+      </c>
+      <c r="C334">
+        <v>1892</v>
+      </c>
+      <c r="P334" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="335" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>231</v>
+      </c>
+      <c r="B335">
+        <v>95</v>
+      </c>
+      <c r="C335">
+        <v>1892</v>
+      </c>
+      <c r="P335" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="336" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>218</v>
+      </c>
+      <c r="B336">
+        <v>95</v>
+      </c>
+      <c r="C336">
+        <v>1892</v>
+      </c>
+      <c r="P336" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="337" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>57</v>
+      </c>
+      <c r="B337">
+        <v>96</v>
+      </c>
+      <c r="C337">
+        <v>1892</v>
+      </c>
+      <c r="P337" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="338" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>64</v>
+      </c>
+      <c r="B338">
+        <v>96</v>
+      </c>
+      <c r="C338">
+        <v>1892</v>
+      </c>
+      <c r="P338" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="339" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>184</v>
+      </c>
+      <c r="B339">
+        <v>97</v>
+      </c>
+      <c r="C339">
+        <v>1893</v>
+      </c>
+      <c r="P339" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="340" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>209</v>
+      </c>
+      <c r="B340">
+        <v>97</v>
+      </c>
+      <c r="C340">
+        <v>1893</v>
+      </c>
+      <c r="P340" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="341" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>53</v>
+      </c>
+      <c r="B341">
+        <v>98</v>
+      </c>
+      <c r="C341">
+        <v>1893</v>
+      </c>
+      <c r="P341" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="342" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>44</v>
+      </c>
+      <c r="B342">
+        <v>98</v>
+      </c>
+      <c r="C342">
+        <v>1894</v>
+      </c>
+      <c r="P342" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="343" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>55</v>
+      </c>
+      <c r="B343">
+        <v>99</v>
+      </c>
+      <c r="C343">
+        <v>1894</v>
+      </c>
+      <c r="P343" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="344" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>59</v>
+      </c>
+      <c r="B344">
+        <v>99</v>
+      </c>
+      <c r="C344">
+        <v>1894</v>
+      </c>
+      <c r="P344" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="345" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>231</v>
+      </c>
+      <c r="B345">
+        <v>100</v>
+      </c>
+      <c r="C345">
+        <v>1895</v>
+      </c>
+      <c r="P345" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="346" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>212</v>
+      </c>
+      <c r="B346">
+        <v>100</v>
+      </c>
+      <c r="C346">
+        <v>1895</v>
+      </c>
+      <c r="P346" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="347" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>57</v>
+      </c>
+      <c r="B347">
+        <v>101</v>
+      </c>
+      <c r="C347">
+        <v>1895</v>
+      </c>
+      <c r="P347" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="348" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>248</v>
+      </c>
+      <c r="B348">
+        <v>101</v>
+      </c>
+      <c r="C348">
+        <v>1895</v>
+      </c>
+      <c r="P348" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="349" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>249</v>
+      </c>
+      <c r="B349">
+        <v>103</v>
+      </c>
+      <c r="C349">
+        <v>1895</v>
+      </c>
+      <c r="D349" t="s">
+        <v>49</v>
+      </c>
+      <c r="E349" t="s">
+        <v>74</v>
+      </c>
+      <c r="F349" t="s">
+        <v>48</v>
+      </c>
+      <c r="G349" t="s">
+        <v>50</v>
+      </c>
+      <c r="I349" t="s">
+        <v>251</v>
+      </c>
+      <c r="J349" t="s">
+        <v>252</v>
+      </c>
+      <c r="K349" t="s">
+        <v>146</v>
+      </c>
+      <c r="L349" t="s">
+        <v>250</v>
+      </c>
+      <c r="P349" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="350" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>64</v>
+      </c>
+      <c r="B350">
+        <v>104</v>
+      </c>
+      <c r="C350">
+        <v>1895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Afegides dades Baptismes Blancafort
</commit_message>
<xml_diff>
--- a/Bisbats/Catalunya/Lleida/Blancafort/Sacraments/Baptismes/Excel/Baptismes_Parroquia_Blancafort.xlsx
+++ b/Bisbats/Catalunya/Lleida/Blancafort/Sacraments/Baptismes/Excel/Baptismes_Parroquia_Blancafort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vstudio-code\repositorisArbre\DadesGenerals\Bisbats\Catalunya\Lleida\Blancafort\Sacraments\Baptismes\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E7D78B-ADA5-46EE-8FDB-015885FF2210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C319A09-4856-4445-B22C-ECA5B9132D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="329">
   <si>
     <t>Cognoms</t>
   </si>
@@ -931,6 +931,90 @@
   </si>
   <si>
     <t>Aran Pedra</t>
+  </si>
+  <si>
+    <t>Gessé Queralt</t>
+  </si>
+  <si>
+    <t>Gessé Taribó</t>
+  </si>
+  <si>
+    <t>Domingo Pedra</t>
+  </si>
+  <si>
+    <t>06/05/1851</t>
+  </si>
+  <si>
+    <t>Gessé Gessé Joseph Liberato Ramon</t>
+  </si>
+  <si>
+    <t>Joseph Gessé i Rita Marquet</t>
+  </si>
+  <si>
+    <t>Jaume Gessé Marquet</t>
+  </si>
+  <si>
+    <t>Thomas Gessé i Rita Marquet</t>
+  </si>
+  <si>
+    <t>Joseph Gessé</t>
+  </si>
+  <si>
+    <t>Rosa Cortés</t>
+  </si>
+  <si>
+    <t>Vicenta Gessé Marquet</t>
+  </si>
+  <si>
+    <t>Badia Cortés</t>
+  </si>
+  <si>
+    <t>2 Quinque Libri 1750-1831</t>
+  </si>
+  <si>
+    <t>Jubillà</t>
+  </si>
+  <si>
+    <t>Seufenís?</t>
+  </si>
+  <si>
+    <t>Terés</t>
+  </si>
+  <si>
+    <t>Gessé</t>
+  </si>
+  <si>
+    <t>Castells</t>
+  </si>
+  <si>
+    <t>Badia</t>
+  </si>
+  <si>
+    <t>Gessé Amat</t>
+  </si>
+  <si>
+    <t>Ferrer Molins</t>
+  </si>
+  <si>
+    <t>Badia Oliva</t>
+  </si>
+  <si>
+    <t>Castells Mas</t>
+  </si>
+  <si>
+    <t>Porta</t>
+  </si>
+  <si>
+    <t>Farré</t>
+  </si>
+  <si>
+    <t>Molins Gessé</t>
+  </si>
+  <si>
+    <t>Castells Hospital</t>
+  </si>
+  <si>
+    <t>Terés Flores</t>
   </si>
 </sst>
 </file>
@@ -1265,11 +1349,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q436"/>
+  <dimension ref="A1:Q477"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A411" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A437" sqref="A437"/>
+      <pane ySplit="1" topLeftCell="A445" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A478" sqref="A478"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8131,7 +8215,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="433" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>128</v>
       </c>
@@ -8141,8 +8225,11 @@
       <c r="C433">
         <v>1849</v>
       </c>
-    </row>
-    <row r="434" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P433" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="434" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>114</v>
       </c>
@@ -8152,8 +8239,11 @@
       <c r="C434">
         <v>1849</v>
       </c>
-    </row>
-    <row r="435" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P434" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="435" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>115</v>
       </c>
@@ -8163,8 +8253,11 @@
       <c r="C435">
         <v>1849</v>
       </c>
-    </row>
-    <row r="436" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P435" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="436" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>124</v>
       </c>
@@ -8173,6 +8266,526 @@
       </c>
       <c r="C436">
         <v>1850</v>
+      </c>
+      <c r="P436" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="437" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>301</v>
+      </c>
+      <c r="B437">
+        <v>23</v>
+      </c>
+      <c r="C437">
+        <v>1850</v>
+      </c>
+      <c r="P437" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="438" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
+        <v>120</v>
+      </c>
+      <c r="B438">
+        <v>23</v>
+      </c>
+      <c r="C438">
+        <v>1850</v>
+      </c>
+      <c r="P438" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="439" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>302</v>
+      </c>
+      <c r="B439">
+        <v>23</v>
+      </c>
+      <c r="C439">
+        <v>1850</v>
+      </c>
+      <c r="P439" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="440" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>303</v>
+      </c>
+      <c r="B440">
+        <v>23</v>
+      </c>
+      <c r="C440">
+        <v>1850</v>
+      </c>
+      <c r="P440" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="441" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>125</v>
+      </c>
+      <c r="B441">
+        <v>23</v>
+      </c>
+      <c r="C441">
+        <v>1851</v>
+      </c>
+      <c r="P441" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="442" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>305</v>
+      </c>
+      <c r="B442">
+        <v>24</v>
+      </c>
+      <c r="C442">
+        <v>1851</v>
+      </c>
+      <c r="D442" t="s">
+        <v>307</v>
+      </c>
+      <c r="E442" t="s">
+        <v>311</v>
+      </c>
+      <c r="F442" t="s">
+        <v>306</v>
+      </c>
+      <c r="G442" t="s">
+        <v>308</v>
+      </c>
+      <c r="I442" t="s">
+        <v>304</v>
+      </c>
+      <c r="J442" t="s">
+        <v>309</v>
+      </c>
+      <c r="K442" t="s">
+        <v>310</v>
+      </c>
+      <c r="L442" t="s">
+        <v>304</v>
+      </c>
+      <c r="P442" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="443" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>126</v>
+      </c>
+      <c r="B443">
+        <v>24</v>
+      </c>
+      <c r="C443">
+        <v>1851</v>
+      </c>
+      <c r="P443" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="444" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>124</v>
+      </c>
+      <c r="B444">
+        <v>24</v>
+      </c>
+      <c r="C444">
+        <v>1851</v>
+      </c>
+      <c r="P444" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="445" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>122</v>
+      </c>
+      <c r="B445">
+        <v>25</v>
+      </c>
+      <c r="C445">
+        <v>1851</v>
+      </c>
+      <c r="P445" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="446" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>103</v>
+      </c>
+      <c r="B446">
+        <v>25</v>
+      </c>
+      <c r="C446">
+        <v>1851</v>
+      </c>
+      <c r="P446" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="447" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>130</v>
+      </c>
+      <c r="B447">
+        <v>25</v>
+      </c>
+      <c r="C447">
+        <v>1851</v>
+      </c>
+      <c r="P447" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="448" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A448" t="s">
+        <v>55</v>
+      </c>
+      <c r="B448">
+        <v>26</v>
+      </c>
+      <c r="C448">
+        <v>1851</v>
+      </c>
+      <c r="P448" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="449" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>312</v>
+      </c>
+      <c r="B449">
+        <v>26</v>
+      </c>
+      <c r="C449">
+        <v>1852</v>
+      </c>
+      <c r="P449" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="450" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A450" t="s">
+        <v>315</v>
+      </c>
+      <c r="B450">
+        <v>1</v>
+      </c>
+      <c r="C450">
+        <v>1737</v>
+      </c>
+      <c r="P450" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="451" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>314</v>
+      </c>
+      <c r="B451">
+        <v>1</v>
+      </c>
+      <c r="C451">
+        <v>1737</v>
+      </c>
+    </row>
+    <row r="452" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>316</v>
+      </c>
+      <c r="B452">
+        <v>1</v>
+      </c>
+      <c r="C452">
+        <v>1737</v>
+      </c>
+    </row>
+    <row r="453" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
+        <v>317</v>
+      </c>
+      <c r="B453">
+        <v>2</v>
+      </c>
+      <c r="C453">
+        <v>1738</v>
+      </c>
+    </row>
+    <row r="454" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
+        <v>318</v>
+      </c>
+      <c r="B454">
+        <v>2</v>
+      </c>
+      <c r="C454">
+        <v>1738</v>
+      </c>
+    </row>
+    <row r="455" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>317</v>
+      </c>
+      <c r="B455">
+        <v>2</v>
+      </c>
+      <c r="C455">
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="456" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>314</v>
+      </c>
+      <c r="B456">
+        <v>3</v>
+      </c>
+      <c r="C456">
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="457" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>317</v>
+      </c>
+      <c r="B457">
+        <v>3</v>
+      </c>
+      <c r="C457">
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="458" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>318</v>
+      </c>
+      <c r="B458">
+        <v>3</v>
+      </c>
+      <c r="C458">
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="459" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>319</v>
+      </c>
+      <c r="B459">
+        <v>4</v>
+      </c>
+      <c r="C459">
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="460" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>316</v>
+      </c>
+      <c r="B460">
+        <v>4</v>
+      </c>
+      <c r="C460">
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="461" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>318</v>
+      </c>
+      <c r="B461">
+        <v>4</v>
+      </c>
+      <c r="C461">
+        <v>1741</v>
+      </c>
+    </row>
+    <row r="462" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>319</v>
+      </c>
+      <c r="B462">
+        <v>5</v>
+      </c>
+      <c r="C462">
+        <v>1742</v>
+      </c>
+    </row>
+    <row r="463" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>314</v>
+      </c>
+      <c r="B463">
+        <v>5</v>
+      </c>
+      <c r="C463">
+        <v>1742</v>
+      </c>
+    </row>
+    <row r="464" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>320</v>
+      </c>
+      <c r="B464">
+        <v>5</v>
+      </c>
+      <c r="C464">
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="465" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>321</v>
+      </c>
+      <c r="B465">
+        <v>6</v>
+      </c>
+      <c r="C465">
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="466" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>322</v>
+      </c>
+      <c r="B466">
+        <v>6</v>
+      </c>
+      <c r="C466">
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="467" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>323</v>
+      </c>
+      <c r="B467">
+        <v>6</v>
+      </c>
+      <c r="C467">
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="468" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>314</v>
+      </c>
+      <c r="B468">
+        <v>7</v>
+      </c>
+      <c r="C468">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="469" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>324</v>
+      </c>
+      <c r="B469">
+        <v>7</v>
+      </c>
+      <c r="C469">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="470" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>323</v>
+      </c>
+      <c r="B470">
+        <v>8</v>
+      </c>
+      <c r="C470">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="471" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>325</v>
+      </c>
+      <c r="B471">
+        <v>8</v>
+      </c>
+      <c r="C471">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="472" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>325</v>
+      </c>
+      <c r="B472">
+        <v>8</v>
+      </c>
+      <c r="C472">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="473" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>323</v>
+      </c>
+      <c r="B473">
+        <v>9</v>
+      </c>
+      <c r="C473">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="474" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>324</v>
+      </c>
+      <c r="B474">
+        <v>9</v>
+      </c>
+      <c r="C474">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="475" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>326</v>
+      </c>
+      <c r="B475">
+        <v>10</v>
+      </c>
+      <c r="C475">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="476" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>327</v>
+      </c>
+      <c r="B476">
+        <v>10</v>
+      </c>
+      <c r="C476">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="477" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
+        <v>328</v>
+      </c>
+      <c r="B477">
+        <v>10</v>
+      </c>
+      <c r="C477">
+        <v>1748</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
afegint dades indexades blancafort
</commit_message>
<xml_diff>
--- a/Bisbats/Catalunya/Lleida/Blancafort/Sacraments/Baptismes/Excel/Baptismes_Parroquia_Blancafort.xlsx
+++ b/Bisbats/Catalunya/Lleida/Blancafort/Sacraments/Baptismes/Excel/Baptismes_Parroquia_Blancafort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vstudio-code\repositorisArbre\DadesGenerals\Bisbats\Catalunya\Lleida\Blancafort\Sacraments\Baptismes\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C319A09-4856-4445-B22C-ECA5B9132D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5078EB-4F9F-462C-8972-CE6E116F2FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="361">
   <si>
     <t>Cognoms</t>
   </si>
@@ -1015,6 +1015,102 @@
   </si>
   <si>
     <t>Terés Flores</t>
+  </si>
+  <si>
+    <t>Jubullà Hospital</t>
+  </si>
+  <si>
+    <t>Mas Gessé</t>
+  </si>
+  <si>
+    <t>Gessé Fondevila</t>
+  </si>
+  <si>
+    <t>Camarasa Gessé</t>
+  </si>
+  <si>
+    <t>Farré Amat</t>
+  </si>
+  <si>
+    <t>Mas Salse</t>
+  </si>
+  <si>
+    <t>Hospital Nadal</t>
+  </si>
+  <si>
+    <t>Jubillà Hospital</t>
+  </si>
+  <si>
+    <t>Gessé Cirès</t>
+  </si>
+  <si>
+    <t>Molins Gese</t>
+  </si>
+  <si>
+    <t>Terés Lloret</t>
+  </si>
+  <si>
+    <t>Mas Soro?</t>
+  </si>
+  <si>
+    <t>Jubillà Farré</t>
+  </si>
+  <si>
+    <t>Mauri Moltò</t>
+  </si>
+  <si>
+    <t>Gessé Pérez</t>
+  </si>
+  <si>
+    <t>Mas Castells</t>
+  </si>
+  <si>
+    <t>Gessé Subira</t>
+  </si>
+  <si>
+    <t>Badia Pasqual</t>
+  </si>
+  <si>
+    <t>Jesinto Gessé Polo</t>
+  </si>
+  <si>
+    <t>03/02/1762</t>
+  </si>
+  <si>
+    <t>Concordia Gessé (Donsella) (Tia)</t>
+  </si>
+  <si>
+    <t>Thomàs Gessé (Moso) (Oncle)</t>
+  </si>
+  <si>
+    <t>Gessé Subirà</t>
+  </si>
+  <si>
+    <t>Gessé Perez</t>
+  </si>
+  <si>
+    <t>Borros</t>
+  </si>
+  <si>
+    <t>Gessé ¿?</t>
+  </si>
+  <si>
+    <t>Badia Pérez</t>
+  </si>
+  <si>
+    <t>Gessé Caufapé</t>
+  </si>
+  <si>
+    <t>Isabet Caufapé</t>
+  </si>
+  <si>
+    <t>Gessé Caufapé Maria Isabet Blasia</t>
+  </si>
+  <si>
+    <t>Gessé Fontdevila</t>
+  </si>
+  <si>
+    <t>Gessé Subirada</t>
   </si>
 </sst>
 </file>
@@ -1349,11 +1445,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q477"/>
+  <dimension ref="A1:Q570"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A445" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A478" sqref="A478"/>
+      <pane ySplit="1" topLeftCell="A550" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A571" sqref="A571"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8788,6 +8884,1053 @@
         <v>1748</v>
       </c>
     </row>
+    <row r="478" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>329</v>
+      </c>
+      <c r="B478">
+        <v>11</v>
+      </c>
+      <c r="C478">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="479" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>330</v>
+      </c>
+      <c r="B479">
+        <v>11</v>
+      </c>
+      <c r="C479">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="480" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>331</v>
+      </c>
+      <c r="B480">
+        <v>11</v>
+      </c>
+      <c r="C480">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="481" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>332</v>
+      </c>
+      <c r="B481">
+        <v>11</v>
+      </c>
+      <c r="C481">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="482" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>333</v>
+      </c>
+      <c r="B482">
+        <v>12</v>
+      </c>
+      <c r="C482">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="483" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
+        <v>151</v>
+      </c>
+      <c r="B483">
+        <v>12</v>
+      </c>
+      <c r="C483">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="484" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>334</v>
+      </c>
+      <c r="B484">
+        <v>12</v>
+      </c>
+      <c r="C484">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="485" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>182</v>
+      </c>
+      <c r="B485">
+        <v>13</v>
+      </c>
+      <c r="C485">
+        <v>1749</v>
+      </c>
+      <c r="Q485" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="486" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>327</v>
+      </c>
+      <c r="B486">
+        <v>13</v>
+      </c>
+      <c r="C486">
+        <v>1750</v>
+      </c>
+      <c r="Q486" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="487" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>335</v>
+      </c>
+      <c r="B487">
+        <v>13</v>
+      </c>
+      <c r="C487">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="488" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>323</v>
+      </c>
+      <c r="B488">
+        <v>14</v>
+      </c>
+      <c r="C488">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="489" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
+        <v>336</v>
+      </c>
+      <c r="B489">
+        <v>14</v>
+      </c>
+      <c r="C489">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="490" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A490" t="s">
+        <v>337</v>
+      </c>
+      <c r="B490">
+        <v>14</v>
+      </c>
+      <c r="C490">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="491" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>332</v>
+      </c>
+      <c r="B491">
+        <v>14</v>
+      </c>
+      <c r="C491">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="492" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>338</v>
+      </c>
+      <c r="B492">
+        <v>15</v>
+      </c>
+      <c r="C492">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="493" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>334</v>
+      </c>
+      <c r="B493">
+        <v>15</v>
+      </c>
+      <c r="C493">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="494" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A494" t="s">
+        <v>331</v>
+      </c>
+      <c r="B494">
+        <v>15</v>
+      </c>
+      <c r="C494">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="495" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>330</v>
+      </c>
+      <c r="B495">
+        <v>15</v>
+      </c>
+      <c r="C495">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="496" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>339</v>
+      </c>
+      <c r="B496">
+        <v>16</v>
+      </c>
+      <c r="C496">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="497" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>324</v>
+      </c>
+      <c r="B497">
+        <v>16</v>
+      </c>
+      <c r="C497">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="498" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
+        <v>340</v>
+      </c>
+      <c r="B498">
+        <v>16</v>
+      </c>
+      <c r="C498">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="499" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
+        <v>335</v>
+      </c>
+      <c r="B499">
+        <v>16</v>
+      </c>
+      <c r="C499">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="500" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>331</v>
+      </c>
+      <c r="B500">
+        <v>17</v>
+      </c>
+      <c r="C500">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="501" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A501" t="s">
+        <v>327</v>
+      </c>
+      <c r="B501">
+        <v>17</v>
+      </c>
+      <c r="C501">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="502" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A502" t="s">
+        <v>316</v>
+      </c>
+      <c r="B502">
+        <v>17</v>
+      </c>
+      <c r="C502">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="503" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
+        <v>335</v>
+      </c>
+      <c r="B503">
+        <v>18</v>
+      </c>
+      <c r="C503">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="504" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A504" t="s">
+        <v>323</v>
+      </c>
+      <c r="B504">
+        <v>18</v>
+      </c>
+      <c r="C504">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="505" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A505" t="s">
+        <v>182</v>
+      </c>
+      <c r="B505">
+        <v>18</v>
+      </c>
+      <c r="C505">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="506" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A506" t="s">
+        <v>332</v>
+      </c>
+      <c r="B506">
+        <v>18</v>
+      </c>
+      <c r="C506">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="507" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A507" t="s">
+        <v>341</v>
+      </c>
+      <c r="B507">
+        <v>19</v>
+      </c>
+      <c r="C507">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="508" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A508" t="s">
+        <v>334</v>
+      </c>
+      <c r="B508">
+        <v>19</v>
+      </c>
+      <c r="C508">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="509" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A509" t="s">
+        <v>335</v>
+      </c>
+      <c r="B509">
+        <v>19</v>
+      </c>
+      <c r="C509">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="510" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A510" t="s">
+        <v>330</v>
+      </c>
+      <c r="B510">
+        <v>20</v>
+      </c>
+      <c r="C510">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="511" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A511" t="s">
+        <v>332</v>
+      </c>
+      <c r="B511">
+        <v>20</v>
+      </c>
+      <c r="C511">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="512" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A512" t="s">
+        <v>326</v>
+      </c>
+      <c r="B512">
+        <v>20</v>
+      </c>
+      <c r="C512">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="513" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A513" t="s">
+        <v>182</v>
+      </c>
+      <c r="B513">
+        <v>21</v>
+      </c>
+      <c r="C513">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="514" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A514" t="s">
+        <v>327</v>
+      </c>
+      <c r="B514">
+        <v>21</v>
+      </c>
+      <c r="C514">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="515" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
+        <v>331</v>
+      </c>
+      <c r="B515">
+        <v>21</v>
+      </c>
+      <c r="C515">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="516" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A516" t="s">
+        <v>342</v>
+      </c>
+      <c r="B516">
+        <v>21</v>
+      </c>
+      <c r="C516">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="517" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A517" t="s">
+        <v>332</v>
+      </c>
+      <c r="B517">
+        <v>22</v>
+      </c>
+      <c r="C517">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="518" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A518" t="s">
+        <v>339</v>
+      </c>
+      <c r="B518">
+        <v>22</v>
+      </c>
+      <c r="C518">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="519" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A519" t="s">
+        <v>341</v>
+      </c>
+      <c r="B519">
+        <v>22</v>
+      </c>
+      <c r="C519">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="520" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A520" t="s">
+        <v>335</v>
+      </c>
+      <c r="B520">
+        <v>22</v>
+      </c>
+      <c r="C520">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="521" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A521" t="s">
+        <v>331</v>
+      </c>
+      <c r="B521">
+        <v>23</v>
+      </c>
+      <c r="C521">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="522" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A522" t="s">
+        <v>343</v>
+      </c>
+      <c r="B522">
+        <v>23</v>
+      </c>
+      <c r="C522">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="523" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A523" t="s">
+        <v>344</v>
+      </c>
+      <c r="B523">
+        <v>23</v>
+      </c>
+      <c r="C523">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="524" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A524" t="s">
+        <v>334</v>
+      </c>
+      <c r="B524">
+        <v>23</v>
+      </c>
+      <c r="C524">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="525" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A525" t="s">
+        <v>335</v>
+      </c>
+      <c r="B525">
+        <v>24</v>
+      </c>
+      <c r="C525">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="526" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A526" t="s">
+        <v>182</v>
+      </c>
+      <c r="B526">
+        <v>24</v>
+      </c>
+      <c r="C526">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="527" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A527" t="s">
+        <v>330</v>
+      </c>
+      <c r="B527">
+        <v>24</v>
+      </c>
+      <c r="C527">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="528" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A528" t="s">
+        <v>124</v>
+      </c>
+      <c r="B528">
+        <v>24</v>
+      </c>
+      <c r="C528">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="529" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A529" t="s">
+        <v>327</v>
+      </c>
+      <c r="B529">
+        <v>24</v>
+      </c>
+      <c r="C529">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="530" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A530" t="s">
+        <v>341</v>
+      </c>
+      <c r="B530">
+        <v>25</v>
+      </c>
+      <c r="C530">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="531" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A531" t="s">
+        <v>332</v>
+      </c>
+      <c r="B531">
+        <v>25</v>
+      </c>
+      <c r="C531">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="532" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A532" t="s">
+        <v>343</v>
+      </c>
+      <c r="B532">
+        <v>25</v>
+      </c>
+      <c r="C532">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="533" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A533" t="s">
+        <v>335</v>
+      </c>
+      <c r="B533">
+        <v>25</v>
+      </c>
+      <c r="C533">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="534" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A534" t="s">
+        <v>339</v>
+      </c>
+      <c r="B534">
+        <v>26</v>
+      </c>
+      <c r="C534">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="535" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A535" t="s">
+        <v>344</v>
+      </c>
+      <c r="B535">
+        <v>26</v>
+      </c>
+      <c r="C535">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="536" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A536" t="s">
+        <v>332</v>
+      </c>
+      <c r="B536">
+        <v>26</v>
+      </c>
+      <c r="C536">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="537" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A537" t="s">
+        <v>334</v>
+      </c>
+      <c r="B537">
+        <v>27</v>
+      </c>
+      <c r="C537">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="538" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A538" t="s">
+        <v>331</v>
+      </c>
+      <c r="B538">
+        <v>27</v>
+      </c>
+      <c r="C538">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="539" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A539" t="s">
+        <v>345</v>
+      </c>
+      <c r="B539">
+        <v>27</v>
+      </c>
+      <c r="C539">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="540" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A540" t="s">
+        <v>330</v>
+      </c>
+      <c r="B540">
+        <v>27</v>
+      </c>
+      <c r="C540">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="541" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A541" t="s">
+        <v>182</v>
+      </c>
+      <c r="B541">
+        <v>28</v>
+      </c>
+      <c r="C541">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="542" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A542" t="s">
+        <v>341</v>
+      </c>
+      <c r="B542">
+        <v>28</v>
+      </c>
+      <c r="C542">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="543" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A543" t="s">
+        <v>124</v>
+      </c>
+      <c r="B543">
+        <v>28</v>
+      </c>
+      <c r="C543">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="544" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A544" t="s">
+        <v>332</v>
+      </c>
+      <c r="B544">
+        <v>28</v>
+      </c>
+      <c r="C544">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="545" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A545" t="s">
+        <v>335</v>
+      </c>
+      <c r="B545">
+        <v>29</v>
+      </c>
+      <c r="C545">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="546" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A546" t="s">
+        <v>346</v>
+      </c>
+      <c r="B546">
+        <v>29</v>
+      </c>
+      <c r="C546">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="547" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A547" t="s">
+        <v>344</v>
+      </c>
+      <c r="B547">
+        <v>29</v>
+      </c>
+      <c r="C547">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="548" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A548" t="s">
+        <v>327</v>
+      </c>
+      <c r="B548">
+        <v>29</v>
+      </c>
+      <c r="C548">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="549" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A549" t="s">
+        <v>339</v>
+      </c>
+      <c r="B549">
+        <v>30</v>
+      </c>
+      <c r="C549">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="550" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A550" t="s">
+        <v>341</v>
+      </c>
+      <c r="B550">
+        <v>30</v>
+      </c>
+      <c r="C550">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="551" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A551" t="s">
+        <v>358</v>
+      </c>
+      <c r="B551">
+        <v>30</v>
+      </c>
+      <c r="C551">
+        <v>1761</v>
+      </c>
+      <c r="D551" t="s">
+        <v>347</v>
+      </c>
+      <c r="E551" t="s">
+        <v>357</v>
+      </c>
+      <c r="J551" t="s">
+        <v>350</v>
+      </c>
+      <c r="K551" t="s">
+        <v>349</v>
+      </c>
+      <c r="L551" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="552" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A552" t="s">
+        <v>334</v>
+      </c>
+      <c r="B552">
+        <v>30</v>
+      </c>
+      <c r="C552">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="553" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A553" t="s">
+        <v>351</v>
+      </c>
+      <c r="B553">
+        <v>31</v>
+      </c>
+      <c r="C553">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="554" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A554" t="s">
+        <v>332</v>
+      </c>
+      <c r="B554">
+        <v>31</v>
+      </c>
+      <c r="C554">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="555" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A555" t="s">
+        <v>352</v>
+      </c>
+      <c r="B555">
+        <v>31</v>
+      </c>
+      <c r="C555">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="556" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A556" t="s">
+        <v>330</v>
+      </c>
+      <c r="B556">
+        <v>32</v>
+      </c>
+      <c r="C556">
+        <v>1762</v>
+      </c>
+      <c r="Q556" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="557" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A557" t="s">
+        <v>182</v>
+      </c>
+      <c r="B557">
+        <v>32</v>
+      </c>
+      <c r="C557">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="558" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A558" t="s">
+        <v>354</v>
+      </c>
+      <c r="B558">
+        <v>32</v>
+      </c>
+      <c r="C558">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="559" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A559" t="s">
+        <v>355</v>
+      </c>
+      <c r="B559">
+        <v>32</v>
+      </c>
+      <c r="C559">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="560" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A560" t="s">
+        <v>356</v>
+      </c>
+      <c r="B560">
+        <v>33</v>
+      </c>
+      <c r="C560">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="561" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A561" t="s">
+        <v>344</v>
+      </c>
+      <c r="B561">
+        <v>33</v>
+      </c>
+      <c r="C561">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="562" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A562" t="s">
+        <v>359</v>
+      </c>
+      <c r="B562">
+        <v>34</v>
+      </c>
+      <c r="C562">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="563" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A563" t="s">
+        <v>332</v>
+      </c>
+      <c r="B563">
+        <v>34</v>
+      </c>
+      <c r="C563">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="564" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A564" t="s">
+        <v>335</v>
+      </c>
+      <c r="B564">
+        <v>34</v>
+      </c>
+      <c r="C564">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="565" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A565" t="s">
+        <v>334</v>
+      </c>
+      <c r="B565">
+        <v>34</v>
+      </c>
+      <c r="C565">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="566" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A566" t="s">
+        <v>341</v>
+      </c>
+      <c r="B566">
+        <v>35</v>
+      </c>
+      <c r="C566">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="567" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A567" t="s">
+        <v>332</v>
+      </c>
+      <c r="B567">
+        <v>35</v>
+      </c>
+      <c r="C567">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="568" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A568" t="s">
+        <v>356</v>
+      </c>
+      <c r="B568">
+        <v>36</v>
+      </c>
+      <c r="C568">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="569" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A569" t="s">
+        <v>360</v>
+      </c>
+      <c r="B569">
+        <v>36</v>
+      </c>
+      <c r="C569">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="570" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A570" t="s">
+        <v>343</v>
+      </c>
+      <c r="B570">
+        <v>36</v>
+      </c>
+      <c r="C570">
+        <v>1764</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:Q350" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>